<commit_message>
Going through dev mode settings, discovering CLEAR SCREEN AND COLOURS CAN BE A THING
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="4110"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="662">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -1912,9 +1912,6 @@
     <t>360 min/6 hr</t>
   </si>
   <si>
-    <t>1 - 1.5 hr searching through different text parsers/developers and whiteboarding</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 - 3.5 hr Searching through IF packages/called authoring systems. Found Python and Non-python ones. Needs lots of time for this investigation. </t>
   </si>
   <si>
@@ -1955,38 +1952,6 @@
 2.0 Understand Liam's Algorithm 
 2.0 Modify to read in image
 3.0 Get printing based on dynamic inputs and sizing from settings and integrate into code</t>
-  </si>
-  <si>
-    <t>* Inventory similar but all Text
-*5.0 No Ascii art (or at least size of the consol), no sounds/music, stats,
-* Also revoke nonsense content and updates
-* DO NOT BREAK IMMERSION
-*1.0 Enter dev mode by typing 420E69 into the setting screen
-*0.5 Only show info that is if you're in dev mode
-Only have saving as a developer.
-*0.5 Put you into Tyler Kashak but don't make that your name, name is Doug but is in Tyler Kashak mode which can still be accessed by Typing it in
-*3.0 Maybe either hide settings file OR make it identified by something else (Naming of a file?)
-*1.0 See if renaming files messes anything up or can keep low level hiding
-*3.0 For game saves have it so it saves after you attack someone so can't reload attack. Also game saves when you hit exit. You can still get around that by copying your game file but I don't think there's any way to get around that. (Easy encryption, renaming, and hiding files) 
-*3.0 for health and other stats just say: "You feel injured", "weak", "broken", "great"etc 
-For attack just have "you feel strong!", "You're basically god", but don't have too much precision 
-Use if statement delimeters
-*2.0 quest flag hitter from Consol in Devmode with quest keyword (type in name of quest) (implement like other keyword dictionary lookup)
-*0.5 Devmode option name to play as just doug and not Tyler Kashak
- *4.0 Maybe option to set stats, spawn weapons, Enemies, etc
-*0.5 Make it a seperate extended set of acceptable verbs so you can't even say those commands in normal play
-It's basically just creative mode at that point</t>
-  </si>
-  <si>
-    <t>* In GUI window have options to save/load game, pause, volume settings, window size, text size, colour settings maybe?
-* These settings are saved locally to the game file
-* For 0.30.0 
-3.0 Make an interface that is in game and also at the start
-Have it just extend the gamesettings dictionary and implement with: 
-1.0 pause (pauses game time), 
-5.0 window size that shows print limits in both directions (x and y) (affects ascii art, gives suggestion on console size and lets you increase or decrease text per line for printer), 
-If you have this will have to have a min window size for some fixed displays
-1.0 feedback (link), disclaimer (same one), credits (same as ending)</t>
   </si>
   <si>
     <t>SUPER nice-tohave/non-prirority, LOTS of interface work</t>
@@ -2283,6 +2248,192 @@
   </si>
   <si>
     <t>7 - 3 hrs  Alpha 0.30.0 Breaking down, integrating Notes, limits, detailed, ACTUAL FEATURE LOCK AND SCHEUDULE! Time to start!</t>
+  </si>
+  <si>
+    <t>14 -</t>
+  </si>
+  <si>
+    <t>15 -</t>
+  </si>
+  <si>
+    <t>16 -</t>
+  </si>
+  <si>
+    <t>17 -</t>
+  </si>
+  <si>
+    <t>OCT 1 - 1.5 hr searching through different text parsers/developers and whiteboarding</t>
+  </si>
+  <si>
+    <t>18 -</t>
+  </si>
+  <si>
+    <t>19 -</t>
+  </si>
+  <si>
+    <t>20 -</t>
+  </si>
+  <si>
+    <t>21 -</t>
+  </si>
+  <si>
+    <t>22 -</t>
+  </si>
+  <si>
+    <t>23 -</t>
+  </si>
+  <si>
+    <t>24 -</t>
+  </si>
+  <si>
+    <t>25 -</t>
+  </si>
+  <si>
+    <t>26 -</t>
+  </si>
+  <si>
+    <t>27 -</t>
+  </si>
+  <si>
+    <t>29 -</t>
+  </si>
+  <si>
+    <t>31 -</t>
+  </si>
+  <si>
+    <t>NOV 1 -</t>
+  </si>
+  <si>
+    <t>2 -</t>
+  </si>
+  <si>
+    <t>3 -</t>
+  </si>
+  <si>
+    <t>4 -</t>
+  </si>
+  <si>
+    <t>5 -</t>
+  </si>
+  <si>
+    <t>6 -</t>
+  </si>
+  <si>
+    <t>7 -</t>
+  </si>
+  <si>
+    <t>Oct 7 -</t>
+  </si>
+  <si>
+    <t>Pygame Learning</t>
+  </si>
+  <si>
+    <t>28 -</t>
+  </si>
+  <si>
+    <t>30 -</t>
+  </si>
+  <si>
+    <t>9 - ✔ Learning framework display and events</t>
+  </si>
+  <si>
+    <t>8 -X</t>
+  </si>
+  <si>
+    <t>9 - 1.5 hrs removing music/sound, info, stats, and setting up dev keywords</t>
+  </si>
+  <si>
+    <t>* In GUI window have options to save/load game, pause, text speed, volume settings, window size, text size, colour settings maybe?
+* These settings are saved locally to the game file
+* For 0.30.0 
+3.0 Make an interface that is in game and also at the start
+Have it just extend the gamesettings dictionary and implement with: 
+1.0 pause (pauses game time), 
+5.0 window size that shows print limits in both directions (x and y) (affects ascii art, gives suggestion on console size and lets you increase or decrease text per line for printer), 
+If you have this will have to have a min window size for some fixed displays
+1.0 feedback (link), disclaimer (same one), credits (same as ending)</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Good Looking</t>
+  </si>
+  <si>
+    <t>Anyone</t>
+  </si>
+  <si>
+    <t>*1.0 See if renaming files messes anything up or can keep low level hiding
+*3.0 For game saves have it so it saves after you attack someone so can't reload attack. Also game saves when you hit exit. You can still get around that by copying your game file but I don't think there's any way to get around that. (Easy encryption, renaming, and hiding files) 
+python how to make a hidden folder
+https://stackoverflow.com/questions/549109/hide-folders-file-with-python
+https://code.activestate.com/recipes/303343/
+https://docs.microsoft.com/en-us/windows/win32/api/fileapi/nf-fileapi-setfileattributesa?redirectedfrom=MSDN
+https://www.daniweb.com/programming/software-development/threads/180031/how-to-hide-a-file-using-python
+*3.0 for health and other stats just say: "You feel injured", "weak", "broken", "great"etc 
+For attack just have "you feel strong!", "You're basically god", but don't have too much precision 
+Use if statement delimeters
+*2.0 quest flag hitter from Consol in Devmode with quest keyword (type in name of quest) (implement like other keyword dictionary lookup)
+*0.5 Devmode option name to play as just doug and not Tyler Kashak
+ *4.0 Maybe option to set stats, spawn weapons, Enemies, etc
+*0.5 Make it a seperate extended set of acceptable verbs so you can't even say those commands in normal play
+It's basically just creative mode at that point
+Nice to Have:
+* "You've unlocked the POWER of the '/' KEY. You now have the power to modify your world as you see fit.\nUse it wisely." You enable devmode with all the creative functions once you beat the game ( don't have it write DevMode to gamesettings as want it local to file and still not to be discovered)
+* Any multi-line inputs need '/' and gets put into creativemode script
+setting paramters of all types ex) /setEnemy Dr. Minnick sinfo "Dogs are not hogs"
+Ability to create new default items/characters in your location /createEnemy
+Ability to read out all object attributes, maybe later see specific ones with /seeEnemy Dr. Minnick sinfo
+Done:
+* Redact INFO/Art/Music/Map
+REMOVED No Ascii art (or at least until is dynamicl), no stats (stats, attack things, inspecting), music/sounds, map
+NOTE PAP, 10:30 left in there for the MEME but not further implemented
+CHANGED Only shows times if you're on speedrun mode!
+NOTE DO NOT BREAK IMMERSION
+* Dev Mode
+ADDED Can only use certain keywords in DevMode
+CHANGED Devmode make it automatically be fast test and disables openning
+ADDED Enter dev mode by typing 420E69 into Setting screen (say nothing), or ingame have it say "YOU dont' understand that command"
+Before running the game DevMode in setting.ini will need to be disabled being written in settingscreen AND command
+REMOVED devmode from setting Screen
+REMOVED         self.item = None  from ENEMY class
+ADDED Only show info that is if you're in dev mode including info from enemies and inspectibles
+CHANGED DevMode Doesn't make your name Tyler Kashak, makes it Doug Fallon so you don't discover.</t>
+  </si>
+  <si>
+    <t>10 - 2.5 Going through dev mode settings, discovering CLEAR SCREEN AND COLOURS CAN BE A THING</t>
+  </si>
+  <si>
+    <t>10 - ✔ Learned colouring, rectangles, some key events, and basic framework of moving objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 - Next is trying renaming files for obsurity, windows file hiding, command creative mode, and looking more/defining more </t>
+  </si>
+  <si>
+    <t>Found out you can clear screen, colour, maybe even change font size
+Using colourize module utilizing ANSI escape coding
+This means not only text background and forground can be done (probably through printT/writing characters
+BUT YOU CAN CLEAR THE SCREEN WHICH MEANS ANIMATIONS AND UPDATING SCREENS
+Might be concern you may want to be able to go back and read things. IDK
+This also means screen can probably read out characters one by one...
+Also never considered possibility of having MULTIPLE text terminals (might need to open ports?)
+https://www.devdungeon.com/content/colorize-terminal-output-python
+https://stackoverflow.com/questions/3592673/change-console-font-in-windows
+https://en.wikipedia.org/wiki/ANSI_escape_code#DOS_and_Windows
+https://liferay.dev/blogs/-/blogs/enable-ansi-colors-in-windows-command-prompt
+Still to investigate:
+python change terminal font
+pythong change terminal bold
+python change terminal background picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I like this structure of learning/looking through next thing while working on the thing before! </t>
+  </si>
+  <si>
+    <t>Might be able to keep up through INFORM, Zombie Modding, and Unity</t>
+  </si>
+  <si>
+    <t>Constantly need to find a good learning source though</t>
   </si>
 </sst>
 </file>
@@ -2420,7 +2571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2465,9 +2616,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2480,6 +2628,12 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2684,10 +2838,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I61" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A4:I61"/>
-  <sortState ref="A5:I61">
-    <sortCondition ref="G4:G61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I62" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A4:I62"/>
+  <sortState ref="A5:I62">
+    <sortCondition ref="A4:A62"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Feature"/>
@@ -3005,10 +3159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,25 +3346,25 @@
         <v>527</v>
       </c>
       <c r="B13" t="s">
+        <v>623</v>
+      </c>
+      <c r="C13" t="s">
         <v>530</v>
       </c>
-      <c r="C13" t="s">
-        <v>531</v>
-      </c>
       <c r="D13" t="s">
+        <v>552</v>
+      </c>
+      <c r="E13" t="s">
+        <v>554</v>
+      </c>
+      <c r="F13" t="s">
         <v>555</v>
       </c>
-      <c r="E13" t="s">
-        <v>557</v>
-      </c>
-      <c r="F13" t="s">
-        <v>558</v>
-      </c>
       <c r="G13" t="s">
+        <v>553</v>
+      </c>
+      <c r="H13" t="s">
         <v>556</v>
-      </c>
-      <c r="H13" t="s">
-        <v>559</v>
       </c>
       <c r="I13" t="s">
         <v>421</v>
@@ -3218,28 +3372,323 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>618</v>
+      </c>
+      <c r="B14" t="s">
+        <v>648</v>
+      </c>
+      <c r="C14" t="s">
+        <v>649</v>
+      </c>
+      <c r="D14" t="s">
+        <v>655</v>
+      </c>
+      <c r="E14" t="s">
+        <v>657</v>
+      </c>
+      <c r="F14" t="s">
+        <v>549</v>
+      </c>
+      <c r="G14" t="s">
+        <v>550</v>
+      </c>
+      <c r="I14" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>619</v>
+      </c>
+      <c r="B15" t="s">
+        <v>620</v>
+      </c>
+      <c r="C15" t="s">
         <v>621</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D15" t="s">
+        <v>622</v>
+      </c>
+      <c r="E15" t="s">
+        <v>624</v>
+      </c>
+      <c r="F15" t="s">
+        <v>625</v>
+      </c>
+      <c r="G15" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>627</v>
+      </c>
+      <c r="B16" t="s">
+        <v>628</v>
+      </c>
+      <c r="C16" t="s">
+        <v>629</v>
+      </c>
+      <c r="D16" t="s">
+        <v>630</v>
+      </c>
+      <c r="E16" t="s">
+        <v>631</v>
+      </c>
+      <c r="F16" t="s">
+        <v>632</v>
+      </c>
+      <c r="G16" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>645</v>
+      </c>
+      <c r="B17" t="s">
+        <v>634</v>
+      </c>
+      <c r="C17" t="s">
+        <v>646</v>
+      </c>
+      <c r="D17" t="s">
+        <v>635</v>
+      </c>
+      <c r="E17" t="s">
+        <v>636</v>
+      </c>
+      <c r="F17" t="s">
+        <v>637</v>
+      </c>
+      <c r="G17" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>639</v>
+      </c>
+      <c r="B18" t="s">
+        <v>640</v>
+      </c>
+      <c r="C18" t="s">
+        <v>641</v>
+      </c>
+      <c r="D18" t="s">
+        <v>642</v>
+      </c>
+      <c r="E18" t="s">
+        <v>546</v>
+      </c>
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>548</v>
+      </c>
+      <c r="B19" t="s">
         <v>549</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C19" t="s">
+        <v>550</v>
+      </c>
+      <c r="D19" t="s">
+        <v>619</v>
+      </c>
+      <c r="E19" t="s">
+        <v>620</v>
+      </c>
+      <c r="F19" t="s">
+        <v>621</v>
+      </c>
+      <c r="G19" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>643</v>
+      </c>
+      <c r="B29" t="s">
+        <v>546</v>
+      </c>
+      <c r="C29" t="s">
+        <v>647</v>
+      </c>
+      <c r="D29" t="s">
+        <v>656</v>
+      </c>
+      <c r="E29" t="s">
+        <v>548</v>
+      </c>
+      <c r="F29" t="s">
+        <v>549</v>
+      </c>
+      <c r="G29" t="s">
+        <v>550</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>619</v>
+      </c>
+      <c r="B30" t="s">
+        <v>620</v>
+      </c>
+      <c r="C30" t="s">
+        <v>621</v>
+      </c>
+      <c r="D30" t="s">
+        <v>622</v>
+      </c>
+      <c r="E30" t="s">
+        <v>624</v>
+      </c>
+      <c r="F30" t="s">
+        <v>625</v>
+      </c>
+      <c r="G30" t="s">
+        <v>626</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>627</v>
+      </c>
+      <c r="B31" t="s">
+        <v>628</v>
+      </c>
+      <c r="C31" t="s">
+        <v>629</v>
+      </c>
+      <c r="D31" t="s">
+        <v>630</v>
+      </c>
+      <c r="E31" t="s">
+        <v>631</v>
+      </c>
+      <c r="F31" t="s">
+        <v>632</v>
+      </c>
+      <c r="G31" t="s">
+        <v>633</v>
+      </c>
+      <c r="I31" s="9">
+        <v>45</v>
+      </c>
+      <c r="J31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>645</v>
+      </c>
+      <c r="B32" t="s">
+        <v>634</v>
+      </c>
+      <c r="C32" t="s">
+        <v>646</v>
+      </c>
+      <c r="D32" t="s">
+        <v>635</v>
+      </c>
+      <c r="E32" t="s">
+        <v>636</v>
+      </c>
+      <c r="F32" t="s">
+        <v>637</v>
+      </c>
+      <c r="G32" t="s">
+        <v>638</v>
+      </c>
+      <c r="I32" t="s">
+        <v>459</v>
+      </c>
+      <c r="J32" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>639</v>
+      </c>
+      <c r="B33" t="s">
+        <v>640</v>
+      </c>
+      <c r="C33" t="s">
+        <v>641</v>
+      </c>
+      <c r="D33" t="s">
+        <v>642</v>
+      </c>
+      <c r="E33" t="s">
+        <v>546</v>
+      </c>
+      <c r="F33" t="s">
         <v>97</v>
       </c>
-      <c r="D14" t="s">
+      <c r="G33" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>548</v>
+      </c>
+      <c r="B34" t="s">
+        <v>549</v>
+      </c>
+      <c r="C34" t="s">
         <v>550</v>
       </c>
-      <c r="E14" t="s">
-        <v>551</v>
-      </c>
-      <c r="F14" t="s">
-        <v>552</v>
-      </c>
-      <c r="G14" t="s">
-        <v>553</v>
-      </c>
-      <c r="I14" t="s">
-        <v>554</v>
+      <c r="D34" t="s">
+        <v>619</v>
+      </c>
+      <c r="E34" t="s">
+        <v>620</v>
+      </c>
+      <c r="F34" t="s">
+        <v>621</v>
+      </c>
+      <c r="G34" t="s">
+        <v>622</v>
+      </c>
+      <c r="H34" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -4281,8 +4730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E15"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4310,7 +4759,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4356,22 +4805,31 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
+        <v>520</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>411</v>
+        <v>79</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G5" t="s">
-        <v>503</v>
+        <v>458</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" t="s">
+        <v>82</v>
       </c>
       <c r="K5" s="22" t="s">
         <v>519</v>
@@ -4391,22 +4849,28 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E6" t="s">
-        <v>324</v>
+        <v>81</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>410</v>
+        <v>357</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>503</v>
+        <v>380</v>
+      </c>
+      <c r="H6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" t="s">
+        <v>87</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>515</v>
@@ -4426,28 +4890,31 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>516</v>
       </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
       <c r="D7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>305</v>
+        <v>359</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>503</v>
+        <v>380</v>
       </c>
       <c r="H7" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="I7" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>516</v>
@@ -4466,30 +4933,29 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>21</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>516</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11">
+      <c r="A8">
         <v>4</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>503</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>165</v>
+      <c r="B8" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>356</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>517</v>
@@ -4509,28 +4975,28 @@
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>361</v>
+        <v>532</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>503</v>
       </c>
       <c r="H9" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="I9" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>518</v>
@@ -4550,28 +5016,28 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>48</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>516</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>517</v>
       </c>
       <c r="D10" t="s">
-        <v>469</v>
+        <v>366</v>
       </c>
       <c r="E10" t="s">
-        <v>225</v>
+        <v>108</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>470</v>
+        <v>363</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>503</v>
+        <v>380</v>
       </c>
       <c r="H10" t="s">
-        <v>226</v>
+        <v>109</v>
       </c>
       <c r="I10" t="s">
-        <v>227</v>
+        <v>110</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>520</v>
@@ -4591,25 +5057,31 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>55</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="D11">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
       </c>
       <c r="E11" t="s">
-        <v>468</v>
+        <v>58</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>503</v>
+        <v>380</v>
       </c>
       <c r="H11" t="s">
-        <v>457</v>
+        <v>113</v>
+      </c>
+      <c r="I11" t="s">
+        <v>114</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -4617,31 +5089,31 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>25</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>518</v>
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>520</v>
       </c>
       <c r="C12" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
+        <v>119</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>208</v>
+        <v>117</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>539</v>
+        <v>303</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>503</v>
+        <v>121</v>
       </c>
       <c r="H12" t="s">
-        <v>218</v>
+        <v>122</v>
       </c>
       <c r="I12" t="s">
-        <v>219</v>
+        <v>128</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>76</v>
@@ -4652,28 +5124,31 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>56</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>517</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
       </c>
       <c r="D13" t="s">
-        <v>532</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>569</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>572</v>
+        <v>124</v>
+      </c>
+      <c r="F13" t="s">
+        <v>304</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>503</v>
+        <v>123</v>
       </c>
       <c r="H13" t="s">
-        <v>461</v>
+        <v>126</v>
       </c>
       <c r="I13" t="s">
-        <v>462</v>
+        <v>127</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -4681,28 +5156,28 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>518</v>
+        <v>10</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>517</v>
       </c>
       <c r="D14">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>182</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>533</v>
+        <v>472</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>503</v>
+        <v>380</v>
       </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="I14" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -4710,701 +5185,700 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="C15" t="s">
-        <v>176</v>
+        <v>520</v>
       </c>
       <c r="D15" t="s">
-        <v>511</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
-        <v>507</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>510</v>
+        <v>132</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>473</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>503</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>163</v>
+        <v>134</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" t="s">
+        <v>139</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
-        <v>18</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>518</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="27">
-        <v>20</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>525</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>568</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>504</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="I16" s="27" t="s">
-        <v>160</v>
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="D16" t="s">
+        <v>412</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="H16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
-        <v>50</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>518</v>
+        <v>13</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>517</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>371</v>
+        <v>137</v>
       </c>
       <c r="D17" s="23">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>506</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>537</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>505</v>
-      </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+        <v>136</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>471</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>516</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="C18" t="s">
+        <v>143</v>
       </c>
       <c r="D18">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>380</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="I18" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>380</v>
+        <v>134</v>
       </c>
       <c r="H19" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>517</v>
-      </c>
-      <c r="D20" t="s">
-        <v>366</v>
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>380</v>
+        <v>503</v>
       </c>
       <c r="H20" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="I20" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>517</v>
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>520</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>351</v>
       </c>
       <c r="D21" t="s">
         <v>111</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>534</v>
+        <v>354</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>380</v>
+        <v>156</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>10</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>517</v>
-      </c>
-      <c r="D22">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>182</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>472</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="H22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I22" t="s">
-        <v>130</v>
+      <c r="A22" s="26">
+        <v>18</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="26">
+        <v>20</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>525</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>565</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>12</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>517</v>
-      </c>
-      <c r="D23" t="s">
-        <v>412</v>
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>509</v>
+        <v>306</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>380</v>
       </c>
       <c r="H23" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="I23" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>13</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>517</v>
-      </c>
-      <c r="C24" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D24" t="s">
+        <v>167</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>471</v>
+        <v>164</v>
+      </c>
+      <c r="F24" t="s">
+        <v>307</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>380</v>
+        <v>120</v>
       </c>
       <c r="H24" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="I24" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>14</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>517</v>
-      </c>
-      <c r="C25" t="s">
-        <v>143</v>
-      </c>
-      <c r="D25">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>362</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="H25" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" t="s">
-        <v>152</v>
+      <c r="A25" s="11">
+        <v>21</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11">
+        <v>4</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>517</v>
-      </c>
-      <c r="C26" t="s">
-        <v>135</v>
-      </c>
-      <c r="D26" t="s">
-        <v>220</v>
+        <v>22</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>308</v>
+        <v>361</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>222</v>
+        <v>503</v>
+      </c>
+      <c r="H26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I26" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27">
-        <v>7</v>
+        <v>243</v>
+      </c>
+      <c r="D27" t="s">
+        <v>214</v>
       </c>
       <c r="E27" t="s">
-        <v>368</v>
-      </c>
-      <c r="F27" t="s">
-        <v>369</v>
+        <v>206</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>328</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>260</v>
+        <v>121</v>
+      </c>
+      <c r="H27" t="s">
+        <v>213</v>
+      </c>
+      <c r="I27" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
+      </c>
+      <c r="C28" t="s">
+        <v>142</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>356</v>
+        <v>207</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>364</v>
+        <v>310</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>380</v>
+        <v>215</v>
       </c>
       <c r="H28" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="I28" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>518</v>
       </c>
+      <c r="C29" t="s">
+        <v>258</v>
+      </c>
       <c r="D29">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>306</v>
+        <v>650</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>380</v>
+        <v>503</v>
       </c>
       <c r="H29" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="I29" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>34</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>518</v>
+        <v>26</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>517</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30">
-        <v>6</v>
+        <v>135</v>
+      </c>
+      <c r="D30" t="s">
+        <v>220</v>
       </c>
       <c r="E30" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>456</v>
+        <v>308</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>380</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>114</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D31" t="s">
-        <v>111</v>
+      <c r="D31">
+        <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>436</v>
+        <v>202</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>440</v>
+        <v>309</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="H31" t="s">
-        <v>438</v>
-      </c>
-      <c r="I31" t="s">
-        <v>439</v>
+        <v>215</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
+      </c>
+      <c r="C32" t="s">
+        <v>176</v>
       </c>
       <c r="D32" t="s">
-        <v>167</v>
+        <v>511</v>
       </c>
       <c r="E32" t="s">
-        <v>164</v>
-      </c>
-      <c r="F32" t="s">
-        <v>307</v>
+        <v>507</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>510</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H32" t="s">
-        <v>166</v>
-      </c>
-      <c r="I32" t="s">
-        <v>165</v>
+        <v>503</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D33" t="s">
-        <v>133</v>
+      <c r="D33">
+        <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>473</v>
+        <v>177</v>
+      </c>
+      <c r="F33" t="s">
+        <v>311</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="H33" t="s">
-        <v>138</v>
-      </c>
-      <c r="I33" t="s">
-        <v>139</v>
+      <c r="H33" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>520</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
+        <v>231</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>360</v>
+        <v>312</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H34" t="s">
-        <v>146</v>
-      </c>
-      <c r="I34" t="s">
-        <v>151</v>
+        <v>230</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>520</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>177</v>
-      </c>
-      <c r="F35" t="s">
-        <v>311</v>
+        <v>302</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>313</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>134</v>
+        <v>234</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>114</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C36" t="s">
-        <v>119</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
+      <c r="D36">
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>303</v>
+        <v>350</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H36" t="s">
-        <v>122</v>
-      </c>
-      <c r="I36" t="s">
-        <v>128</v>
+        <v>238</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C37" t="s">
-        <v>243</v>
-      </c>
-      <c r="D37" t="s">
-        <v>214</v>
+      <c r="D37">
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H37" t="s">
-        <v>213</v>
-      </c>
-      <c r="I37" t="s">
-        <v>212</v>
+        <v>240</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C38" t="s">
-        <v>231</v>
+        <v>142</v>
       </c>
       <c r="D38">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>312</v>
+        <v>456</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>230</v>
+        <v>380</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>233</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>520</v>
       </c>
       <c r="C39" t="s">
-        <v>351</v>
-      </c>
-      <c r="D39" t="s">
-        <v>111</v>
+        <v>243</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>354</v>
+        <v>314</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="H39" t="s">
-        <v>157</v>
-      </c>
-      <c r="I39" t="s">
-        <v>158</v>
+        <v>244</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>520</v>
@@ -5412,20 +5886,23 @@
       <c r="C40" t="s">
         <v>243</v>
       </c>
+      <c r="D40">
+        <v>20</v>
+      </c>
       <c r="E40" t="s">
-        <v>351</v>
+        <v>186</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="G40" t="s">
-        <v>156</v>
-      </c>
-      <c r="H40" t="s">
-        <v>353</v>
-      </c>
-      <c r="I40" t="s">
-        <v>352</v>
+        <v>345</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -5456,536 +5933,531 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" t="s">
-        <v>118</v>
+        <v>58</v>
+      </c>
+      <c r="D42">
+        <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>124</v>
+        <v>368</v>
       </c>
       <c r="F42" t="s">
-        <v>304</v>
+        <v>369</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="H42" t="s">
-        <v>126</v>
-      </c>
-      <c r="I42" t="s">
-        <v>127</v>
+        <v>380</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D43" t="s">
-        <v>277</v>
+      <c r="D43">
+        <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>571</v>
+        <v>316</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>123</v>
+        <v>252</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>520</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
-      </c>
-      <c r="D44">
-        <v>10</v>
+        <v>267</v>
+      </c>
+      <c r="D44" t="s">
+        <v>266</v>
       </c>
       <c r="E44" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="H44" t="s">
-        <v>216</v>
-      </c>
-      <c r="I44" t="s">
-        <v>217</v>
+        <v>252</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D45">
-        <v>8</v>
+      <c r="C45" t="s">
+        <v>275</v>
+      </c>
+      <c r="D45" t="s">
+        <v>274</v>
       </c>
       <c r="E45" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>223</v>
+        <v>276</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>224</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D46">
-        <v>20</v>
+      <c r="D46" t="s">
+        <v>277</v>
       </c>
       <c r="E46" t="s">
-        <v>302</v>
+        <v>197</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>235</v>
+        <v>278</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>236</v>
+        <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C47" t="s">
-        <v>287</v>
-      </c>
       <c r="D47" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="E47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D48">
-        <v>10</v>
+      <c r="D48" t="s">
+        <v>277</v>
       </c>
       <c r="E48" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>350</v>
+        <v>568</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>238</v>
+        <v>123</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>239</v>
+        <v>282</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>237</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>520</v>
       </c>
       <c r="C49" t="s">
-        <v>243</v>
-      </c>
-      <c r="D49">
-        <v>12</v>
+        <v>287</v>
+      </c>
+      <c r="D49" t="s">
+        <v>284</v>
       </c>
       <c r="E49" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>250</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D50">
-        <v>20</v>
+      <c r="D50" t="s">
+        <v>288</v>
       </c>
       <c r="E50" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>241</v>
+        <v>293</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C51" t="s">
-        <v>243</v>
-      </c>
-      <c r="D51">
-        <v>20</v>
+      <c r="D51" t="s">
+        <v>296</v>
       </c>
       <c r="E51" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>253</v>
+        <v>295</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>254</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D52">
-        <v>10</v>
+        <v>516</v>
+      </c>
+      <c r="D52" t="s">
+        <v>469</v>
       </c>
       <c r="E52" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>316</v>
+        <v>470</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>264</v>
+        <v>503</v>
+      </c>
+      <c r="H52" t="s">
+        <v>226</v>
+      </c>
+      <c r="I52" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C53" t="s">
-        <v>267</v>
-      </c>
       <c r="D53" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E53" t="s">
-        <v>195</v>
+        <v>268</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>317</v>
+        <v>358</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>154</v>
+        <v>521</v>
+      </c>
+      <c r="H53" t="s">
+        <v>271</v>
+      </c>
+      <c r="I53" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="C54" t="s">
-        <v>275</v>
-      </c>
-      <c r="D54" t="s">
-        <v>274</v>
+        <v>515</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>196</v>
+        <v>411</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>273</v>
+        <v>367</v>
+      </c>
+      <c r="G54" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>42</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D55" t="s">
-        <v>277</v>
-      </c>
-      <c r="E55" t="s">
-        <v>197</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="H55" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="I55" s="14" t="s">
-        <v>279</v>
-      </c>
+      <c r="A55" s="26">
+        <v>50</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="D55" s="26">
+        <v>7</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="F55" s="29" t="s">
+        <v>536</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>505</v>
+      </c>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D56" t="s">
-        <v>274</v>
+        <v>515</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>198</v>
+        <v>324</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>320</v>
+        <v>410</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="H56" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>280</v>
+        <v>503</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D57" t="s">
-        <v>288</v>
-      </c>
       <c r="E57" t="s">
-        <v>209</v>
+        <v>341</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="I57" s="14" t="s">
-        <v>289</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D58" t="s">
-        <v>296</v>
+      <c r="C58" t="s">
+        <v>243</v>
       </c>
       <c r="E58" t="s">
-        <v>210</v>
+        <v>351</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="H58" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="I58" s="14" t="s">
-        <v>294</v>
+        <v>355</v>
+      </c>
+      <c r="G58" t="s">
+        <v>156</v>
+      </c>
+      <c r="H58" t="s">
+        <v>353</v>
+      </c>
+      <c r="I58" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>520</v>
       </c>
       <c r="D59" t="s">
-        <v>269</v>
+        <v>111</v>
       </c>
       <c r="E59" t="s">
-        <v>268</v>
+        <v>436</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>358</v>
+        <v>440</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>521</v>
+        <v>437</v>
       </c>
       <c r="H59" t="s">
-        <v>271</v>
+        <v>438</v>
       </c>
       <c r="I59" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="C60" t="s">
-        <v>85</v>
-      </c>
-      <c r="D60" t="s">
-        <v>80</v>
+        <v>516</v>
+      </c>
+      <c r="D60">
+        <v>24</v>
       </c>
       <c r="E60" t="s">
-        <v>79</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>458</v>
+        <v>468</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>654</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>84</v>
+        <v>503</v>
       </c>
       <c r="H60" t="s">
-        <v>83</v>
-      </c>
-      <c r="I60" t="s">
-        <v>82</v>
+        <v>457</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>52</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>520</v>
+        <v>56</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="D61" t="s">
+        <v>531</v>
       </c>
       <c r="E61" t="s">
-        <v>341</v>
+        <v>566</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="G61" s="10"/>
+        <v>569</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="H61" t="s">
+        <v>461</v>
+      </c>
+      <c r="I61" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>57</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D62" t="s">
+        <v>651</v>
+      </c>
+      <c r="F62" s="34" t="s">
+        <v>658</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="H62" t="s">
+        <v>652</v>
+      </c>
+      <c r="I62" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I65" t="s">
@@ -6082,7 +6554,7 @@
     <sortCondition descending="1" ref="O5"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B61">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B62">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -6168,7 +6640,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="J9" t="s">
         <v>446</v>
@@ -6260,10 +6732,10 @@
         <v>441</v>
       </c>
       <c r="D13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>517</v>
@@ -6411,7 +6883,7 @@
         <v>388</v>
       </c>
       <c r="F18" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>7</v>
@@ -6433,14 +6905,14 @@
       <c r="C19" t="s">
         <v>441</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="26">
         <v>20</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="26" t="s">
         <v>525</v>
       </c>
       <c r="F19" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>7</v>
@@ -6469,7 +6941,7 @@
         <v>524</v>
       </c>
       <c r="F20" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>7</v>
@@ -6550,7 +7022,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>7</v>
@@ -6578,7 +7050,7 @@
         <v>516</v>
       </c>
       <c r="D26" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
@@ -6589,10 +7061,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>7</v>
@@ -6614,10 +7086,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
+        <v>541</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>544</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>547</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>7</v>
@@ -6642,10 +7114,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
+        <v>542</v>
+      </c>
+      <c r="D31" t="s">
         <v>545</v>
-      </c>
-      <c r="D31" t="s">
-        <v>548</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>7</v>
@@ -6866,12 +7338,12 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E2" t="s">
         <v>514</v>
@@ -6896,10 +7368,10 @@
       <c r="F3" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="30" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6919,10 +7391,10 @@
       <c r="E4" s="19" t="s">
         <v>463</v>
       </c>
-      <c r="P4" s="32">
+      <c r="P4" s="31">
         <v>24</v>
       </c>
-      <c r="Q4" s="32" t="s">
+      <c r="Q4" s="31" t="s">
         <v>463</v>
       </c>
     </row>
@@ -6942,10 +7414,10 @@
       <c r="E5" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="P5" s="33">
+      <c r="P5" s="32">
         <v>8</v>
       </c>
-      <c r="Q5" s="33" t="s">
+      <c r="Q5" s="32" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6960,16 +7432,16 @@
         <v>441</v>
       </c>
       <c r="D6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>569</v>
-      </c>
-      <c r="P6" s="32" t="s">
-        <v>532</v>
-      </c>
-      <c r="Q6" s="32" t="s">
-        <v>615</v>
+        <v>566</v>
+      </c>
+      <c r="P6" s="31" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q6" s="31" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -6988,37 +7460,37 @@
       <c r="E7" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="P7" s="33">
+      <c r="P7" s="32">
         <v>7</v>
       </c>
-      <c r="Q7" s="33" t="s">
+      <c r="Q7" s="32" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>513</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>515</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>522</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>8</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="31" t="s">
         <v>455</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="31" t="s">
         <v>508</v>
       </c>
-      <c r="P8" s="32">
+      <c r="P8" s="31">
         <v>8</v>
       </c>
-      <c r="Q8" s="32" t="s">
-        <v>616</v>
+      <c r="Q8" s="31" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -7028,7 +7500,7 @@
       <c r="B9" t="s">
         <v>518</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>522</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -7037,39 +7509,39 @@
       <c r="E9" s="19" t="s">
         <v>507</v>
       </c>
-      <c r="P9" s="33" t="s">
+      <c r="P9" s="32" t="s">
         <v>511</v>
       </c>
-      <c r="Q9" s="33" t="s">
-        <v>617</v>
+      <c r="Q9" s="32" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
+      <c r="A10" s="31">
         <v>48</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>516</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="31" t="s">
         <v>446</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="31" t="s">
         <v>469</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="31" t="s">
         <v>231</v>
       </c>
       <c r="H10" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I10" t="s">
-        <v>606</v>
-      </c>
-      <c r="P10" s="32" t="s">
+        <v>603</v>
+      </c>
+      <c r="P10" s="31" t="s">
         <v>469</v>
       </c>
-      <c r="Q10" s="32" t="s">
+      <c r="Q10" s="31" t="s">
         <v>231</v>
       </c>
     </row>
@@ -7090,12 +7562,12 @@
         <v>524</v>
       </c>
       <c r="F11" t="s">
-        <v>536</v>
-      </c>
-      <c r="P11" s="33">
+        <v>535</v>
+      </c>
+      <c r="P11" s="32">
         <v>10</v>
       </c>
-      <c r="Q11" s="33" t="s">
+      <c r="Q11" s="32" t="s">
         <v>208</v>
       </c>
     </row>
@@ -7116,16 +7588,16 @@
         <v>208</v>
       </c>
       <c r="H12" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I12" t="s">
-        <v>608</v>
-      </c>
-      <c r="P12" s="32">
+        <v>605</v>
+      </c>
+      <c r="P12" s="31">
         <v>7</v>
       </c>
-      <c r="Q12" s="32" t="s">
-        <v>618</v>
+      <c r="Q12" s="31" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -7145,13 +7617,13 @@
         <v>388</v>
       </c>
       <c r="F13" t="s">
-        <v>535</v>
-      </c>
-      <c r="P13" s="33">
+        <v>534</v>
+      </c>
+      <c r="P13" s="32">
         <v>20</v>
       </c>
-      <c r="Q13" s="33" t="s">
-        <v>619</v>
+      <c r="Q13" s="32" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -7164,31 +7636,31 @@
       <c r="C14" t="s">
         <v>441</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="26">
         <v>20</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="26" t="s">
         <v>525</v>
       </c>
       <c r="F14" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="H14" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I14" t="s">
-        <v>607</v>
-      </c>
-      <c r="P14" s="34">
+        <v>604</v>
+      </c>
+      <c r="P14" s="33">
         <v>20</v>
       </c>
-      <c r="Q14" s="34" t="s">
-        <v>620</v>
+      <c r="Q14" s="33" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="I16" t="s">
         <v>399</v>
@@ -7205,7 +7677,7 @@
         <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -7213,7 +7685,7 @@
         <v>516</v>
       </c>
       <c r="D18" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I18">
         <f>I17*0.5</f>
@@ -7225,10 +7697,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -7239,15 +7711,15 @@
         <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>541</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>544</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -7260,10 +7732,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
+        <v>542</v>
+      </c>
+      <c r="D23" t="s">
         <v>545</v>
-      </c>
-      <c r="D23" t="s">
-        <v>548</v>
       </c>
       <c r="I23" t="s">
         <v>401</v>
@@ -7282,7 +7754,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="I25">
         <v>5</v>
@@ -7312,7 +7784,7 @@
         <v>60</v>
       </c>
       <c r="J28" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -7332,10 +7804,10 @@
         <v>447</v>
       </c>
       <c r="B30" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C30" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="I30">
         <f>I29+I28</f>
@@ -7347,7 +7819,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B31">
         <v>150</v>
@@ -7362,7 +7834,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B32">
         <v>170</v>
@@ -7374,7 +7846,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B33">
         <v>250</v>
@@ -7384,17 +7856,17 @@
         <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I35" t="s">
         <v>409</v>
@@ -7405,7 +7877,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -7436,7 +7908,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -7475,7 +7947,7 @@
         <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7552,7 +8024,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7573,12 +8045,12 @@
         <v>488</v>
       </c>
       <c r="B7" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B8" t="s">
         <v>485</v>
@@ -7586,23 +8058,23 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B9" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B10" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B11" t="s">
         <v>489</v>
@@ -7610,7 +8082,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B12" t="s">
         <v>490</v>
@@ -7618,23 +8090,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B13" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B15" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B16" t="s">
         <v>491</v>
@@ -7642,31 +8114,31 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B17" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B18" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B19" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B20" t="s">
         <v>493</v>
@@ -7674,7 +8146,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B21" t="s">
         <v>494</v>
@@ -7682,7 +8154,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B22" t="s">
         <v>495</v>
@@ -7710,47 +8182,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of changes due to working on other laptop
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\bflaw\Documents\GitHub\EngPhysAdventure\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="4110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="671">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -957,10 +957,6 @@
   </si>
   <si>
     <t>* Make other players be able to interact, fight, talk to eachother</t>
-  </si>
-  <si>
-    <t>* Making so surroundings of obveous areas print out. 
-* Have lore print first and then title+search around you.</t>
   </si>
   <si>
     <t>* Mini-gamers around area. Not made by me but implemented.
@@ -2274,26 +2270,12 @@
     <t>30 -</t>
   </si>
   <si>
-    <t>9 - ✔ Learning framework display and events</t>
-  </si>
-  <si>
     <t>8 -X</t>
   </si>
   <si>
     <t>9 - 1.5 hrs removing music/sound, info, stats, and setting up dev keywords</t>
   </si>
   <si>
-    <t>* In GUI window have options to save/load game, pause, text speed, volume settings, window size, text size, colour settings maybe?
-* These settings are saved locally to the game file
-* For 0.30.0 
-3.0 Make an interface that is in game and also at the start
-Have it just extend the gamesettings dictionary and implement with: 
-1.0 pause (pauses game time), 
-5.0 window size that shows print limits in both directions (x and y) (affects ascii art, gives suggestion on console size and lets you increase or decrease text per line for printer), 
-If you have this will have to have a min window size for some fixed displays
-1.0 feedback (link), disclaimer (same one), credits (same as ending)</t>
-  </si>
-  <si>
     <t>BD</t>
   </si>
   <si>
@@ -2304,9 +2286,6 @@
   </si>
   <si>
     <t>10 - 2.5 Going through dev mode settings, discovering CLEAR SCREEN AND COLOURS CAN BE A THING</t>
-  </si>
-  <si>
-    <t>10 - ✔ Learned colouring, rectangles, some key events, and basic framework of moving objects</t>
   </si>
   <si>
     <t>Found out you can clear screen, colour, maybe even change font size
@@ -2401,9 +2380,6 @@
   </si>
   <si>
     <t>11 - 2.0 Obsucasting file endings, making save only if you exit, fixing loadgame setting bug, and making cache folder hidden</t>
-  </si>
-  <si>
-    <t>12 - Next is word stat descriptions, command creative mode, and looking more/defining more of the colours/clearing</t>
   </si>
   <si>
     <t>* Word based stats/feellings
@@ -2442,6 +2418,111 @@
   </si>
   <si>
     <t>Hours Documenting (2 hours each)</t>
+  </si>
+  <si>
+    <t>9 - ✔ Learning framework display and events (videos 1-4)</t>
+  </si>
+  <si>
+    <t>10 - ✔ Learned colouring, rectangles, some key events, and basic framework of moving objects (videos 5-8)</t>
+  </si>
+  <si>
+    <t>11 - 0.5 hr Adding FPS and more refined moving (videos 9+10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 - 1.15 working on creativeMode parser and input </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 - </t>
+  </si>
+  <si>
+    <t>16 - 0.5 Writing Dev Documentation</t>
+  </si>
+  <si>
+    <t>675 min/11.25</t>
+  </si>
+  <si>
+    <t>* In GUI window have options to save/load game, pause, text speed, volume settings, window size, text size, colour settings maybe?
+* These settings are saved locally to the game file
+* For 0.30.0 
+3.0 Make an interface that is in game and also at the start
+Have it just extend the gamesettings dictionary and implement with: 
+1.0 pause (pauses game time), 
+5.0 window size that shows print limits in both directions (x and y) (affects ascii art, gives suggestion on console size and lets you increase or decrease text per line for printer), 
+If you have this will have to have a min window size for some fixed displays
+1.0 feedback (link), disclaimer (same one), credits (same as ending)
+* Add option to disable monologue</t>
+  </si>
+  <si>
+    <t>21 - 1.0 Writing up ideas for MEPMUD in the car</t>
+  </si>
+  <si>
+    <t>23 - 3.5 Writing Auto Descriptions and fixing descriptions</t>
+  </si>
+  <si>
+    <t>* Search/look around does the surounding.  Remember
+* *Auto descriptions
+The description can be turned into a more in-depth first time description of the place, item, with more detail
+Search gives the short search function
+Look, or look around gives the long description
+The lore is given again with the remember keyword
+Also have a wait or sleep function that says "time passes"
+Add the iron ring and o the starting area
+Was thinking about adding bench but then would need sit functionality. -&gt; no cause feature lock
+This makes it more like a Zork style game with the thing
+* Nice to have: move around left side arrangement so that there isn't two cootes drives and lines up nicely but whatever for now
+Lot I
+ITB
+Alley
+ETB
+vvv T-13
+University Ave
+* MAP DESCRIPTION OVERHALL
+IF SOMETHING IS MENTIONED IN THE LORE IT NEEDS TO BE IN THERE
+ex) Iron Ring, students, and kipling pranks in the lore/monolouge but not actually around there
+*Auto Surroundings
+Having exit if it's outside an interrior (I like this)
+Maybe ellement of discovery that if discovered will say the name like the map
+COMMONIZE WORDING FOR DIRECTIONS AND ACCEPT ALL DIRECTIONS
+ REAR, beneath, forward, backward, below, above 
+Done:
+* CHANGED The MAP object name is now the printed name in capatalized first letter
+* ADDED Map Name convention
+Names are captalized when defined
+The name is surounded by ~ ~ and all captalized when printed through MAP.search
+No delimters (the), prepositions (in, outside), or qualifying words (very)
+Use direction with reference to areas
+ ex)       Front of Hatch. Behind Art Museum. JHE Lobby
+ NOT example) Outside Hatch. Outside Art Museum. Inside JHE
+ exceptions) THE Phoniex (where it's a name)
+Just very basic name of the word that you would want to read quickly
+* CHANGED Added line break at top of each of the function so EACH TURN IS DELIMITED
+MAIN LOOP NOW
+Ask what you want to do
+linebreak
+interpruts what you need to do and calls the function
+Checks any triggers for quests or events
+Checks if the player is alive and it exits the main loop
+* CHANGED Description Layout
+1. MAP Name
+2. IF First time visiting: MAP Lore
+3. ~MAP NAME~
+4. IF FirstOrSecond time visiting: print descriptions (which include search items) (why not add this to the item/person) Else: print short search around you.
+5. Then obvious direction around you
+6. What do you want to do input?
+7. Linebreak 
+* ADDED Basic Auto Surroundings where it searches around you (so far just the quick one)
+Short
+There are _ obveous exits: Left, Right, Front, Back, Up, Down
+[l]eft: _ [r]ight _ [u]p _
+[d]own _ [f]ront [b]ack
+Maybe with the discover mechanic?
+Wordy(default):
+There are _ obveous ways to go: Left, Right, Front, Back, Up, Down
+To your left is _. To your right is _
+Infront of you is _. Behind you is _.
+Upstairs is _. Downstairs is _.
+Maybe with discovery mechanic
+Doesn't need to be wordy, just need to know information - Brian</t>
   </si>
 </sst>
 </file>
@@ -2636,14 +2717,14 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3172,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,7 +3289,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3285,13 +3366,13 @@
         <v>211</v>
       </c>
       <c r="H10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I10" t="s">
+        <v>457</v>
+      </c>
+      <c r="J10" t="s">
         <v>458</v>
-      </c>
-      <c r="J10" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3302,22 +3383,22 @@
         <v>298</v>
       </c>
       <c r="C11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>299</v>
@@ -3325,258 +3406,261 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>372</v>
+      </c>
+      <c r="B12" t="s">
         <v>373</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>374</v>
       </c>
-      <c r="C12" t="s">
-        <v>375</v>
-      </c>
       <c r="D12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F12" t="s">
+        <v>526</v>
+      </c>
+      <c r="G12" t="s">
+        <v>524</v>
+      </c>
+      <c r="H12" t="s">
         <v>527</v>
       </c>
-      <c r="G12" t="s">
-        <v>525</v>
-      </c>
-      <c r="H12" t="s">
-        <v>528</v>
-      </c>
       <c r="I12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D13" t="s">
+        <v>550</v>
+      </c>
+      <c r="E13" t="s">
+        <v>552</v>
+      </c>
+      <c r="F13" t="s">
+        <v>553</v>
+      </c>
+      <c r="G13" t="s">
         <v>551</v>
       </c>
-      <c r="E13" t="s">
-        <v>553</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>554</v>
       </c>
-      <c r="G13" t="s">
-        <v>552</v>
-      </c>
-      <c r="H13" t="s">
-        <v>555</v>
-      </c>
       <c r="I13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B14" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C14" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="F14" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="G14" t="s">
+        <v>664</v>
+      </c>
+      <c r="H14" t="s">
+        <v>666</v>
+      </c>
+      <c r="I14" t="s">
         <v>549</v>
-      </c>
-      <c r="I14" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>616</v>
+      </c>
+      <c r="B15" t="s">
         <v>617</v>
       </c>
-      <c r="B15" t="s">
-        <v>618</v>
-      </c>
       <c r="C15" t="s">
+        <v>665</v>
+      </c>
+      <c r="D15" t="s">
         <v>619</v>
       </c>
-      <c r="D15" t="s">
-        <v>620</v>
-      </c>
       <c r="E15" t="s">
+        <v>621</v>
+      </c>
+      <c r="F15" t="s">
         <v>622</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>623</v>
-      </c>
-      <c r="G15" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>668</v>
+      </c>
+      <c r="B16" t="s">
         <v>625</v>
       </c>
-      <c r="B16" t="s">
-        <v>626</v>
-      </c>
       <c r="C16" t="s">
+        <v>669</v>
+      </c>
+      <c r="D16" t="s">
         <v>627</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>628</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>629</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>630</v>
-      </c>
-      <c r="G16" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>642</v>
+      </c>
+      <c r="B17" t="s">
+        <v>631</v>
+      </c>
+      <c r="C17" t="s">
         <v>643</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>632</v>
       </c>
-      <c r="C17" t="s">
-        <v>644</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>633</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>634</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>635</v>
-      </c>
-      <c r="G17" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>636</v>
+      </c>
+      <c r="B18" t="s">
         <v>637</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>638</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>639</v>
       </c>
-      <c r="D18" t="s">
-        <v>640</v>
-      </c>
       <c r="E18" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F18" t="s">
         <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>546</v>
+      </c>
+      <c r="B19" t="s">
         <v>547</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>548</v>
       </c>
-      <c r="C19" t="s">
-        <v>549</v>
-      </c>
       <c r="D19" t="s">
+        <v>616</v>
+      </c>
+      <c r="E19" t="s">
         <v>617</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>618</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>619</v>
-      </c>
-      <c r="G19" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B29" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C29" t="s">
-        <v>645</v>
+        <v>660</v>
       </c>
       <c r="D29" t="s">
-        <v>653</v>
+        <v>661</v>
       </c>
       <c r="E29" t="s">
+        <v>662</v>
+      </c>
+      <c r="F29" t="s">
         <v>547</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>548</v>
-      </c>
-      <c r="G29" t="s">
-        <v>549</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>616</v>
+      </c>
+      <c r="B30" t="s">
         <v>617</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>618</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>619</v>
       </c>
-      <c r="D30" t="s">
-        <v>620</v>
-      </c>
       <c r="E30" t="s">
+        <v>621</v>
+      </c>
+      <c r="F30" t="s">
         <v>622</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>623</v>
-      </c>
-      <c r="G30" t="s">
-        <v>624</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>15</v>
@@ -3587,25 +3671,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>624</v>
+      </c>
+      <c r="B31" t="s">
         <v>625</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>626</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>627</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>628</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>629</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>630</v>
-      </c>
-      <c r="G31" t="s">
-        <v>631</v>
       </c>
       <c r="I31" s="9">
         <v>45</v>
@@ -3616,90 +3700,90 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>642</v>
+      </c>
+      <c r="B32" t="s">
+        <v>631</v>
+      </c>
+      <c r="C32" t="s">
         <v>643</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>632</v>
       </c>
-      <c r="C32" t="s">
-        <v>644</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>633</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>634</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>635</v>
       </c>
-      <c r="G32" t="s">
-        <v>636</v>
-      </c>
       <c r="I32" t="s">
+        <v>457</v>
+      </c>
+      <c r="J32" t="s">
         <v>458</v>
-      </c>
-      <c r="J32" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>636</v>
+      </c>
+      <c r="B33" t="s">
         <v>637</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>638</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>639</v>
       </c>
-      <c r="D33" t="s">
-        <v>640</v>
-      </c>
       <c r="E33" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F33" t="s">
         <v>97</v>
       </c>
       <c r="G33" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>546</v>
+      </c>
+      <c r="B34" t="s">
         <v>547</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>548</v>
       </c>
-      <c r="C34" t="s">
-        <v>549</v>
-      </c>
       <c r="D34" t="s">
+        <v>616</v>
+      </c>
+      <c r="E34" t="s">
         <v>617</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>618</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>619</v>
       </c>
-      <c r="G34" t="s">
-        <v>620</v>
-      </c>
       <c r="H34" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -3967,7 +4051,7 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>14</v>
@@ -4041,7 +4125,7 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4052,7 +4136,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D15">
         <v>0.28000000000000003</v>
@@ -4095,7 +4179,7 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4149,7 +4233,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -4268,7 +4352,7 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D27">
         <v>0.28999999999999998</v>
@@ -4277,10 +4361,10 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4297,10 +4381,10 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4317,7 +4401,7 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -4334,7 +4418,7 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G30" t="s">
         <v>180</v>
@@ -4462,10 +4546,10 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -4499,7 +4583,7 @@
         <v>4</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4708,7 +4792,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -4741,8 +4825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4770,7 +4854,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4819,7 +4903,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -4828,10 +4912,10 @@
         <v>105</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H5" t="s">
         <v>107</v>
@@ -4840,7 +4924,7 @@
         <v>106</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>72</v>
@@ -4855,12 +4939,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -4868,11 +4952,11 @@
       <c r="E6" t="s">
         <v>148</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>305</v>
+      <c r="F6" s="36" t="s">
+        <v>670</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H6" t="s">
         <v>149</v>
@@ -4881,7 +4965,7 @@
         <v>150</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L6" t="s">
         <v>33</v>
@@ -4901,7 +4985,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11">
@@ -4914,7 +4998,7 @@
         <v>170</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>171</v>
@@ -4923,7 +5007,7 @@
         <v>165</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>19</v>
@@ -4943,7 +5027,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -4952,10 +5036,10 @@
         <v>169</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H8" t="s">
         <v>173</v>
@@ -4964,7 +5048,7 @@
         <v>172</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L8" t="s">
         <v>21</v>
@@ -4984,7 +5068,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C9" t="s">
         <v>258</v>
@@ -4996,10 +5080,10 @@
         <v>208</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>648</v>
+        <v>667</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H9" t="s">
         <v>218</v>
@@ -5008,7 +5092,7 @@
         <v>219</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>18</v>
@@ -5028,22 +5112,22 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C10" t="s">
         <v>176</v>
       </c>
       <c r="D10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>228</v>
@@ -5052,7 +5136,7 @@
         <v>163</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>20</v>
@@ -5072,19 +5156,19 @@
         <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E11" t="s">
         <v>225</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H11" t="s">
         <v>226</v>
@@ -5101,19 +5185,19 @@
         <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>76</v>
@@ -5127,45 +5211,45 @@
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D14">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>467</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>663</v>
+        <v>466</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>658</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -5176,25 +5260,25 @@
         <v>56</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H15" t="s">
+        <v>459</v>
+      </c>
+      <c r="I15" t="s">
         <v>460</v>
-      </c>
-      <c r="I15" t="s">
-        <v>461</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -5205,33 +5289,33 @@
         <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D16" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="E16" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H16" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="I16" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>18</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>517</v>
+      <c r="B17" s="35" t="s">
+        <v>516</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>258</v>
@@ -5240,13 +5324,13 @@
         <v>20</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>159</v>
@@ -5260,22 +5344,22 @@
         <v>50</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D18" s="26">
         <v>7</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
@@ -5285,7 +5369,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D19">
         <v>1.5</v>
@@ -5294,10 +5378,10 @@
         <v>81</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H19" t="s">
         <v>86</v>
@@ -5311,7 +5395,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C20" t="s">
         <v>102</v>
@@ -5323,10 +5407,10 @@
         <v>99</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H20" t="s">
         <v>101</v>
@@ -5340,19 +5424,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H21" t="s">
         <v>103</v>
@@ -5366,19 +5450,19 @@
         <v>6</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E22" t="s">
         <v>108</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H22" t="s">
         <v>109</v>
@@ -5392,7 +5476,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C23" t="s">
         <v>112</v>
@@ -5404,10 +5488,10 @@
         <v>58</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H23" t="s">
         <v>113</v>
@@ -5421,7 +5505,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D24">
         <v>9</v>
@@ -5430,10 +5514,10 @@
         <v>182</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H24" t="s">
         <v>129</v>
@@ -5447,19 +5531,19 @@
         <v>12</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E25" t="s">
         <v>135</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H25" t="s">
         <v>141</v>
@@ -5472,8 +5556,8 @@
       <c r="A26" s="26">
         <v>13</v>
       </c>
-      <c r="B26" s="35" t="s">
-        <v>516</v>
+      <c r="B26" s="34" t="s">
+        <v>515</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>137</v>
@@ -5485,10 +5569,10 @@
         <v>136</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>140</v>
@@ -5502,7 +5586,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C27" t="s">
         <v>143</v>
@@ -5514,10 +5598,10 @@
         <v>142</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H27" t="s">
         <v>144</v>
@@ -5531,7 +5615,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D28">
         <v>8</v>
@@ -5540,10 +5624,10 @@
         <v>161</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H28" t="s">
         <v>162</v>
@@ -5557,7 +5641,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C29" t="s">
         <v>135</v>
@@ -5569,10 +5653,10 @@
         <v>204</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>221</v>
@@ -5586,7 +5670,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C30" t="s">
         <v>142</v>
@@ -5598,10 +5682,10 @@
         <v>184</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>242</v>
@@ -5615,7 +5699,7 @@
         <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
@@ -5624,13 +5708,13 @@
         <v>7</v>
       </c>
       <c r="E31" t="s">
+        <v>367</v>
+      </c>
+      <c r="F31" t="s">
         <v>368</v>
       </c>
-      <c r="F31" t="s">
-        <v>369</v>
-      </c>
       <c r="G31" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H31" s="14" t="s">
         <v>259</v>
@@ -5644,25 +5728,25 @@
         <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D32" t="s">
         <v>111</v>
       </c>
       <c r="E32" t="s">
+        <v>435</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>439</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>440</v>
-      </c>
-      <c r="G32" s="10" t="s">
+      <c r="H32" t="s">
         <v>437</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>438</v>
-      </c>
-      <c r="I32" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -5670,7 +5754,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D33" t="s">
         <v>167</v>
@@ -5679,7 +5763,7 @@
         <v>164</v>
       </c>
       <c r="F33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>120</v>
@@ -5696,7 +5780,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D34" t="s">
         <v>133</v>
@@ -5705,7 +5789,7 @@
         <v>132</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>134</v>
@@ -5722,7 +5806,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C35" t="s">
         <v>147</v>
@@ -5734,7 +5818,7 @@
         <v>145</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>134</v>
@@ -5751,7 +5835,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -5760,7 +5844,7 @@
         <v>177</v>
       </c>
       <c r="F36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>134</v>
@@ -5777,7 +5861,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C37" t="s">
         <v>119</v>
@@ -5806,7 +5890,7 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C38" t="s">
         <v>243</v>
@@ -5818,7 +5902,7 @@
         <v>206</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G38" s="10" t="s">
         <v>121</v>
@@ -5835,7 +5919,7 @@
         <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C39" t="s">
         <v>231</v>
@@ -5847,7 +5931,7 @@
         <v>178</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>230</v>
@@ -5864,10 +5948,10 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C40" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D40" t="s">
         <v>111</v>
@@ -5876,7 +5960,7 @@
         <v>155</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G40" s="10" t="s">
         <v>156</v>
@@ -5893,25 +5977,25 @@
         <v>53</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C41" t="s">
         <v>243</v>
       </c>
       <c r="E41" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G41" t="s">
         <v>156</v>
       </c>
       <c r="H41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I41" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5919,7 +6003,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D42">
         <v>10</v>
@@ -5928,7 +6012,7 @@
         <v>187</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>255</v>
@@ -5945,7 +6029,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C43" t="s">
         <v>125</v>
@@ -5974,7 +6058,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D44" t="s">
         <v>277</v>
@@ -5983,7 +6067,7 @@
         <v>200</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>123</v>
@@ -6000,7 +6084,7 @@
         <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C45" t="s">
         <v>142</v>
@@ -6012,7 +6096,7 @@
         <v>207</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>215</v>
@@ -6029,7 +6113,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D46">
         <v>8</v>
@@ -6038,7 +6122,7 @@
         <v>202</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>215</v>
@@ -6055,7 +6139,7 @@
         <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D47">
         <v>20</v>
@@ -6064,7 +6148,7 @@
         <v>302</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>234</v>
@@ -6081,7 +6165,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C48" t="s">
         <v>287</v>
@@ -6093,7 +6177,7 @@
         <v>201</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>234</v>
@@ -6110,7 +6194,7 @@
         <v>32</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -6119,7 +6203,7 @@
         <v>183</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>238</v>
@@ -6136,7 +6220,7 @@
         <v>35</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C50" t="s">
         <v>243</v>
@@ -6148,7 +6232,7 @@
         <v>185</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>244</v>
@@ -6165,7 +6249,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D51">
         <v>20</v>
@@ -6174,7 +6258,7 @@
         <v>191</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>240</v>
@@ -6191,7 +6275,7 @@
         <v>36</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C52" t="s">
         <v>243</v>
@@ -6203,7 +6287,7 @@
         <v>186</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>252</v>
@@ -6220,7 +6304,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D53">
         <v>10</v>
@@ -6229,7 +6313,7 @@
         <v>189</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>252</v>
@@ -6246,7 +6330,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C54" t="s">
         <v>267</v>
@@ -6258,7 +6342,7 @@
         <v>195</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>252</v>
@@ -6275,7 +6359,7 @@
         <v>41</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C55" t="s">
         <v>275</v>
@@ -6287,7 +6371,7 @@
         <v>196</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>261</v>
@@ -6304,7 +6388,7 @@
         <v>42</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D56" t="s">
         <v>277</v>
@@ -6313,7 +6397,7 @@
         <v>197</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>261</v>
@@ -6330,7 +6414,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D57" t="s">
         <v>274</v>
@@ -6339,7 +6423,7 @@
         <v>198</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>262</v>
@@ -6356,7 +6440,7 @@
         <v>46</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D58" t="s">
         <v>288</v>
@@ -6365,7 +6449,7 @@
         <v>209</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>262</v>
@@ -6382,7 +6466,7 @@
         <v>47</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D59" t="s">
         <v>296</v>
@@ -6391,7 +6475,7 @@
         <v>210</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>263</v>
@@ -6408,7 +6492,7 @@
         <v>49</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D60" t="s">
         <v>269</v>
@@ -6417,10 +6501,10 @@
         <v>268</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H60" t="s">
         <v>271</v>
@@ -6434,7 +6518,7 @@
         <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C61" t="s">
         <v>85</v>
@@ -6446,7 +6530,7 @@
         <v>79</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>84</v>
@@ -6463,29 +6547,29 @@
         <v>52</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E62" t="s">
+        <v>340</v>
+      </c>
+      <c r="F62" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>342</v>
       </c>
       <c r="G62" s="10"/>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I65" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I66" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I67" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.25">
@@ -6493,7 +6577,7 @@
         <v>116</v>
       </c>
       <c r="I68" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.25">
@@ -6501,7 +6585,7 @@
         <v>64</v>
       </c>
       <c r="I69" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.25">
@@ -6509,7 +6593,7 @@
         <v>248</v>
       </c>
       <c r="I70" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.25">
@@ -6517,7 +6601,7 @@
         <v>245</v>
       </c>
       <c r="I71" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.25">
@@ -6527,12 +6611,12 @@
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D73" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D74" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.25">
@@ -6545,7 +6629,7 @@
         <v>247</v>
       </c>
       <c r="F76" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.25">
@@ -6599,140 +6683,140 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
         <v>377</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>378</v>
-      </c>
-      <c r="C2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" t="s">
         <v>380</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>381</v>
-      </c>
-      <c r="C3" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>447</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>448</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C12" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D12" s="19">
         <v>8</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -6740,31 +6824,31 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
+        <v>514</v>
+      </c>
+      <c r="C13" t="s">
+        <v>440</v>
+      </c>
+      <c r="D13" t="s">
+        <v>529</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>515</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H13" t="s">
+        <v>452</v>
+      </c>
+      <c r="I13" t="s">
+        <v>442</v>
+      </c>
+      <c r="J13" t="s">
         <v>441</v>
       </c>
-      <c r="D13" t="s">
-        <v>530</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>565</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>516</v>
-      </c>
-      <c r="H13" t="s">
-        <v>453</v>
-      </c>
-      <c r="I13" t="s">
-        <v>443</v>
-      </c>
-      <c r="J13" t="s">
-        <v>442</v>
-      </c>
       <c r="L13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -6772,28 +6856,28 @@
         <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D14" s="19">
         <v>26</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -6801,10 +6885,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D15" s="19">
         <v>8</v>
@@ -6817,10 +6901,10 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M15" s="20"/>
       <c r="O15" s="20"/>
@@ -6833,13 +6917,13 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>231</v>
@@ -6848,10 +6932,10 @@
         <v>7</v>
       </c>
       <c r="I16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -6859,16 +6943,16 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D17" s="19">
         <v>7</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>7</v>
@@ -6877,7 +6961,7 @@
         <v>7</v>
       </c>
       <c r="J17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -6885,28 +6969,28 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C18" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D18" s="19">
         <v>20</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F18" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -6914,28 +6998,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C19" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D19" s="26">
         <v>20</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J19" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -6943,28 +7027,28 @@
         <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D20" s="19">
         <v>7</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F20" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -6972,10 +7056,10 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C21" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D21" s="19">
         <v>10</v>
@@ -6987,10 +7071,10 @@
         <v>7</v>
       </c>
       <c r="J21" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="L21" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -6998,25 +7082,25 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C22" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L22" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -7027,27 +7111,27 @@
         <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D25">
         <v>8</v>
@@ -7056,29 +7140,29 @@
         <v>7</v>
       </c>
       <c r="L25" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D26" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>7</v>
@@ -7086,7 +7170,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C28" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D28" s="19">
         <v>24</v>
@@ -7095,26 +7179,26 @@
         <v>7</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D30">
         <v>60</v>
@@ -7123,21 +7207,21 @@
         <v>7</v>
       </c>
       <c r="L30" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D31" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -7145,7 +7229,7 @@
         <v>7</v>
       </c>
       <c r="L32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -7153,12 +7237,12 @@
         <v>7</v>
       </c>
       <c r="L33" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>7</v>
@@ -7166,46 +7250,46 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L35" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L36" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L37" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L38" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -7214,29 +7298,29 @@
         <v>7</v>
       </c>
       <c r="L39" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L40" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L41" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -7247,7 +7331,7 @@
         <v>7</v>
       </c>
       <c r="L42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -7274,12 +7358,12 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -7289,12 +7373,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
@@ -7309,12 +7393,12 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -7352,38 +7436,38 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>447</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>448</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P3" s="30" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Q3" s="30" t="s">
         <v>71</v>
@@ -7394,22 +7478,22 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D4" s="19">
         <v>24</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P4" s="31">
         <v>24</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -7417,10 +7501,10 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D5" s="19">
         <v>8</v>
@@ -7440,22 +7524,22 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Q6" s="31" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -7463,48 +7547,48 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D7" s="19">
         <v>7</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="P7" s="32">
         <v>7</v>
       </c>
       <c r="Q7" s="32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D8" s="31">
         <v>8</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="P8" s="31">
         <v>8</v>
       </c>
       <c r="Q8" s="31" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -7512,22 +7596,22 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P9" s="32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q9" s="32" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -7535,25 +7619,25 @@
         <v>48</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>231</v>
       </c>
       <c r="H10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I10" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P10" s="31" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="Q10" s="31" t="s">
         <v>231</v>
@@ -7564,19 +7648,19 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D11" s="19">
         <v>7</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F11" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="P11" s="32">
         <v>10</v>
@@ -7590,10 +7674,10 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D12" s="19">
         <v>10</v>
@@ -7602,16 +7686,16 @@
         <v>208</v>
       </c>
       <c r="H12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P12" s="31">
         <v>7</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -7619,25 +7703,25 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D13" s="19">
         <v>20</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="P13" s="32">
         <v>20</v>
       </c>
       <c r="Q13" s="32" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -7645,44 +7729,44 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D14" s="26">
         <v>20</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H14" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I14" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P14" s="33">
         <v>20</v>
       </c>
       <c r="Q14" s="33" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -7691,54 +7775,54 @@
         <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D18" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I18">
         <f>I17*0.5</f>
         <v>17</v>
       </c>
       <c r="J18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C20" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D20" s="19">
         <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D22">
         <v>60</v>
@@ -7746,13 +7830,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D23" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I23" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -7760,7 +7844,7 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7768,13 +7852,13 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I25">
         <v>5</v>
       </c>
       <c r="J25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -7782,14 +7866,14 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I26">
         <f>I24*4+I25*3</f>
         <v>35</v>
       </c>
       <c r="J26" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -7797,7 +7881,7 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -7806,42 +7890,42 @@
         <v>60</v>
       </c>
       <c r="J28" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I29">
         <f>I25*3*1</f>
         <v>15</v>
       </c>
       <c r="J29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B30" t="s">
+        <v>596</v>
+      </c>
+      <c r="C30" t="s">
         <v>597</v>
-      </c>
-      <c r="C30" t="s">
-        <v>598</v>
       </c>
       <c r="I30">
         <f>I29+I28</f>
         <v>75</v>
       </c>
       <c r="J30" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B31">
         <v>170</v>
@@ -7851,12 +7935,12 @@
         <v>34</v>
       </c>
       <c r="J31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B32">
         <v>190</v>
@@ -7868,7 +7952,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B33">
         <v>270</v>
@@ -7878,20 +7962,20 @@
         <v>54</v>
       </c>
       <c r="I33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I35" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -7899,12 +7983,12 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -7913,7 +7997,7 @@
         <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -7922,20 +8006,20 @@
         <v>42.5</v>
       </c>
       <c r="B41" t="s">
+        <v>418</v>
+      </c>
+      <c r="C41" t="s">
         <v>419</v>
-      </c>
-      <c r="C41" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -7943,7 +8027,7 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -7951,7 +8035,7 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -7960,7 +8044,7 @@
         <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -7969,7 +8053,7 @@
         <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7978,7 +8062,7 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -7987,27 +8071,27 @@
         <v>180</v>
       </c>
       <c r="B52" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -8041,150 +8125,150 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>591</v>
+      </c>
+      <c r="B9" t="s">
         <v>592</v>
-      </c>
-      <c r="B9" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B13" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>594</v>
+      </c>
+      <c r="B18" t="s">
         <v>595</v>
-      </c>
-      <c r="B18" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B21" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B22" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -8204,47 +8288,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish Basic version of auto surroundings, documented, and started playing with compiler
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="672">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2459,12 +2459,9 @@
     <t>23 - 3.5 Writing Auto Descriptions and fixing descriptions</t>
   </si>
   <si>
-    <t>* Search/look around does the surounding.  Remember
-* *Auto descriptions
+    <t>* Improved surroundings
 The description can be turned into a more in-depth first time description of the place, item, with more detail
-Search gives the short search function
 Look, or look around gives the long description
-The lore is given again with the remember keyword
 Also have a wait or sleep function that says "time passes"
 Add the iron ring and o the starting area
 Was thinking about adding bench but then would need sit functionality. -&gt; no cause feature lock
@@ -2522,7 +2519,11 @@
 Infront of you is _. Behind you is _.
 Upstairs is _. Downstairs is _.
 Maybe with discovery mechanic
-Doesn't need to be wordy, just need to know information - Brian</t>
+Doesn't need to be wordy, just need to know information - Brian
+*ADDED Look around now accepted to give search, remember give the lore, wait+sit+sleep to pass time, and die to exit the game</t>
+  </si>
+  <si>
+    <t>24 - 1.25 Finish Basic version of auto surroundings, documented, and started playing with compiler</t>
   </si>
 </sst>
 </file>
@@ -3253,7 +3254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -3525,7 +3526,7 @@
         <v>669</v>
       </c>
       <c r="D16" t="s">
-        <v>627</v>
+        <v>671</v>
       </c>
       <c r="E16" t="s">
         <v>628</v>
@@ -4825,8 +4826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4939,7 +4940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
@@ -4952,7 +4953,7 @@
       <c r="E6" t="s">
         <v>148</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="14" t="s">
         <v>670</v>
       </c>
       <c r="G6" s="10" t="s">
@@ -5022,7 +5023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22</v>
       </c>
@@ -5035,7 +5036,7 @@
       <c r="E8" t="s">
         <v>169</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="36" t="s">
         <v>360</v>
       </c>
       <c r="G8" s="10" t="s">

</xml_diff>

<commit_message>
Compilier done more, nearly there.
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="673">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -1228,14 +1228,6 @@
 * https://docs.python.org/2/tutorial/inputoutput.html - save structured data
 * Update save files so you write or so you understand pickling
 * change the file extensions and names of folders in EBTA to .EBTA or something random (or blank) to hide or obscure files  (make sure it works)</t>
-  </si>
-  <si>
-    <t>* Make so it takes files automatically
-* gives icon automatically 
-* does code checks out 
-* installer gives desktop icon
-* Overwriting old instal to update would be nice.
-* Try changing the file extensions and names of folders in EBTA to .EBTA or something random (or blank) to hide or obscure files (make sure it works first)</t>
   </si>
   <si>
     <t>* Adding time to game. 
@@ -2524,6 +2516,21 @@
   </si>
   <si>
     <t>24 - 1.25 Finish Basic version of auto surroundings, documented, and started playing with compiler</t>
+  </si>
+  <si>
+    <t>* Get the shortcut to not make cache and also for thing to thing
+* does code checks print out
+* Overwriting old instal to update would be nice.
+*remove the build folder and rename the dist folder
+Done:
+*ADDED Make so it takes files/folders automatically when put in includefiles
+How to include files
+https://stackoverflow.com/questions/2553886/how-can-i-bundle-other-files-when-using-cx-freeze
+Needs relative file locations!
+*ADDED Icon populates automatically and Desktop Icon Automatically</t>
+  </si>
+  <si>
+    <t>26 - 1.15 Getting Compilier to go more</t>
   </si>
 </sst>
 </file>
@@ -2661,7 +2668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2723,9 +2730,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3255,7 +3259,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,7 +3294,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3367,13 +3371,13 @@
         <v>211</v>
       </c>
       <c r="H10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I10" t="s">
+        <v>456</v>
+      </c>
+      <c r="J10" t="s">
         <v>457</v>
-      </c>
-      <c r="J10" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3390,16 +3394,16 @@
         <v>347</v>
       </c>
       <c r="E11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>299</v>
@@ -3407,261 +3411,261 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>371</v>
+      </c>
+      <c r="B12" t="s">
         <v>372</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>373</v>
       </c>
-      <c r="C12" t="s">
-        <v>374</v>
-      </c>
       <c r="D12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F12" t="s">
+        <v>525</v>
+      </c>
+      <c r="G12" t="s">
+        <v>523</v>
+      </c>
+      <c r="H12" t="s">
         <v>526</v>
       </c>
-      <c r="G12" t="s">
-        <v>524</v>
-      </c>
-      <c r="H12" t="s">
-        <v>527</v>
-      </c>
       <c r="I12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D13" t="s">
+        <v>549</v>
+      </c>
+      <c r="E13" t="s">
+        <v>551</v>
+      </c>
+      <c r="F13" t="s">
+        <v>552</v>
+      </c>
+      <c r="G13" t="s">
         <v>550</v>
       </c>
-      <c r="E13" t="s">
-        <v>552</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>553</v>
       </c>
-      <c r="G13" t="s">
-        <v>551</v>
-      </c>
-      <c r="H13" t="s">
-        <v>554</v>
-      </c>
       <c r="I13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B14" t="s">
+        <v>643</v>
+      </c>
+      <c r="C14" t="s">
         <v>644</v>
       </c>
-      <c r="C14" t="s">
-        <v>645</v>
-      </c>
       <c r="D14" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F14" t="s">
+        <v>662</v>
+      </c>
+      <c r="G14" t="s">
         <v>663</v>
       </c>
-      <c r="G14" t="s">
-        <v>664</v>
-      </c>
       <c r="H14" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I14" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>615</v>
+      </c>
+      <c r="B15" t="s">
         <v>616</v>
       </c>
-      <c r="B15" t="s">
-        <v>617</v>
-      </c>
       <c r="C15" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D15" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E15" t="s">
+        <v>620</v>
+      </c>
+      <c r="F15" t="s">
         <v>621</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>622</v>
-      </c>
-      <c r="G15" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>667</v>
+      </c>
+      <c r="B16" t="s">
+        <v>624</v>
+      </c>
+      <c r="C16" t="s">
         <v>668</v>
       </c>
-      <c r="B16" t="s">
-        <v>625</v>
-      </c>
-      <c r="C16" t="s">
-        <v>669</v>
-      </c>
       <c r="D16" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E16" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F16" t="s">
+        <v>672</v>
+      </c>
+      <c r="G16" t="s">
         <v>629</v>
-      </c>
-      <c r="G16" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>641</v>
+      </c>
+      <c r="B17" t="s">
+        <v>630</v>
+      </c>
+      <c r="C17" t="s">
         <v>642</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>631</v>
       </c>
-      <c r="C17" t="s">
-        <v>643</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>632</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>633</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>634</v>
-      </c>
-      <c r="G17" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>635</v>
+      </c>
+      <c r="B18" t="s">
         <v>636</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>637</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>638</v>
       </c>
-      <c r="D18" t="s">
-        <v>639</v>
-      </c>
       <c r="E18" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F18" t="s">
         <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>545</v>
+      </c>
+      <c r="B19" t="s">
         <v>546</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>547</v>
       </c>
-      <c r="C19" t="s">
-        <v>548</v>
-      </c>
       <c r="D19" t="s">
+        <v>615</v>
+      </c>
+      <c r="E19" t="s">
         <v>616</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>617</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>618</v>
-      </c>
-      <c r="G19" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B29" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C29" t="s">
+        <v>659</v>
+      </c>
+      <c r="D29" t="s">
         <v>660</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>661</v>
       </c>
-      <c r="E29" t="s">
-        <v>662</v>
-      </c>
       <c r="F29" t="s">
+        <v>546</v>
+      </c>
+      <c r="G29" t="s">
         <v>547</v>
-      </c>
-      <c r="G29" t="s">
-        <v>548</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>615</v>
+      </c>
+      <c r="B30" t="s">
         <v>616</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>617</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>618</v>
       </c>
-      <c r="D30" t="s">
-        <v>619</v>
-      </c>
       <c r="E30" t="s">
+        <v>620</v>
+      </c>
+      <c r="F30" t="s">
         <v>621</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>622</v>
-      </c>
-      <c r="G30" t="s">
-        <v>623</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>15</v>
@@ -3672,25 +3676,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>623</v>
+      </c>
+      <c r="B31" t="s">
         <v>624</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>625</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>626</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>627</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>628</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>629</v>
-      </c>
-      <c r="G31" t="s">
-        <v>630</v>
       </c>
       <c r="I31" s="9">
         <v>45</v>
@@ -3701,90 +3705,90 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>641</v>
+      </c>
+      <c r="B32" t="s">
+        <v>630</v>
+      </c>
+      <c r="C32" t="s">
         <v>642</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>631</v>
       </c>
-      <c r="C32" t="s">
-        <v>643</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>632</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>633</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>634</v>
       </c>
-      <c r="G32" t="s">
-        <v>635</v>
-      </c>
       <c r="I32" t="s">
+        <v>456</v>
+      </c>
+      <c r="J32" t="s">
         <v>457</v>
-      </c>
-      <c r="J32" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>635</v>
+      </c>
+      <c r="B33" t="s">
         <v>636</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>637</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>638</v>
       </c>
-      <c r="D33" t="s">
-        <v>639</v>
-      </c>
       <c r="E33" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F33" t="s">
         <v>97</v>
       </c>
       <c r="G33" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>545</v>
+      </c>
+      <c r="B34" t="s">
         <v>546</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>547</v>
       </c>
-      <c r="C34" t="s">
-        <v>548</v>
-      </c>
       <c r="D34" t="s">
+        <v>615</v>
+      </c>
+      <c r="E34" t="s">
         <v>616</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>617</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>618</v>
       </c>
-      <c r="G34" t="s">
-        <v>619</v>
-      </c>
       <c r="H34" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -4826,7 +4830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C8" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -4855,7 +4859,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4904,7 +4908,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -4913,10 +4917,10 @@
         <v>105</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H5" t="s">
         <v>107</v>
@@ -4925,7 +4929,7 @@
         <v>106</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>72</v>
@@ -4945,7 +4949,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -4954,10 +4958,10 @@
         <v>148</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H6" t="s">
         <v>149</v>
@@ -4966,7 +4970,7 @@
         <v>150</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L6" t="s">
         <v>33</v>
@@ -4986,7 +4990,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11">
@@ -4999,7 +5003,7 @@
         <v>170</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>171</v>
@@ -5008,7 +5012,7 @@
         <v>165</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>19</v>
@@ -5023,12 +5027,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -5036,11 +5040,11 @@
       <c r="E8" t="s">
         <v>169</v>
       </c>
-      <c r="F8" s="36" t="s">
-        <v>360</v>
+      <c r="F8" s="14" t="s">
+        <v>671</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H8" t="s">
         <v>173</v>
@@ -5049,7 +5053,7 @@
         <v>172</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L8" t="s">
         <v>21</v>
@@ -5069,7 +5073,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C9" t="s">
         <v>258</v>
@@ -5081,10 +5085,10 @@
         <v>208</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H9" t="s">
         <v>218</v>
@@ -5093,7 +5097,7 @@
         <v>219</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>18</v>
@@ -5113,22 +5117,22 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C10" t="s">
         <v>176</v>
       </c>
       <c r="D10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>228</v>
@@ -5137,7 +5141,7 @@
         <v>163</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>20</v>
@@ -5157,19 +5161,19 @@
         <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E11" t="s">
         <v>225</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H11" t="s">
         <v>226</v>
@@ -5186,19 +5190,19 @@
         <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>76</v>
@@ -5212,7 +5216,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -5221,10 +5225,10 @@
         <v>323</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -5235,22 +5239,22 @@
         <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D14">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -5261,25 +5265,25 @@
         <v>56</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D15" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E15" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H15" t="s">
+        <v>458</v>
+      </c>
+      <c r="I15" t="s">
         <v>459</v>
-      </c>
-      <c r="I15" t="s">
-        <v>460</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -5290,25 +5294,25 @@
         <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D16" t="s">
+        <v>645</v>
+      </c>
+      <c r="E16" t="s">
+        <v>653</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>649</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="H16" t="s">
         <v>646</v>
       </c>
-      <c r="E16" t="s">
-        <v>654</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>650</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>647</v>
-      </c>
-      <c r="I16" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5316,7 +5320,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>258</v>
@@ -5325,13 +5329,13 @@
         <v>20</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>159</v>
@@ -5345,22 +5349,22 @@
         <v>50</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D18" s="26">
         <v>7</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
@@ -5370,7 +5374,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D19">
         <v>1.5</v>
@@ -5382,7 +5386,7 @@
         <v>356</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H19" t="s">
         <v>86</v>
@@ -5396,7 +5400,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C20" t="s">
         <v>102</v>
@@ -5411,7 +5415,7 @@
         <v>358</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H20" t="s">
         <v>101</v>
@@ -5425,7 +5429,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -5434,10 +5438,10 @@
         <v>355</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H21" t="s">
         <v>103</v>
@@ -5451,19 +5455,19 @@
         <v>6</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E22" t="s">
         <v>108</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H22" t="s">
         <v>109</v>
@@ -5477,7 +5481,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C23" t="s">
         <v>112</v>
@@ -5489,10 +5493,10 @@
         <v>58</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H23" t="s">
         <v>113</v>
@@ -5506,7 +5510,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D24">
         <v>9</v>
@@ -5515,10 +5519,10 @@
         <v>182</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H24" t="s">
         <v>129</v>
@@ -5532,19 +5536,19 @@
         <v>12</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D25" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E25" t="s">
         <v>135</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H25" t="s">
         <v>141</v>
@@ -5558,7 +5562,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>137</v>
@@ -5570,10 +5574,10 @@
         <v>136</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>140</v>
@@ -5587,7 +5591,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C27" t="s">
         <v>143</v>
@@ -5599,10 +5603,10 @@
         <v>142</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H27" t="s">
         <v>144</v>
@@ -5616,7 +5620,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D28">
         <v>8</v>
@@ -5628,7 +5632,7 @@
         <v>305</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H28" t="s">
         <v>162</v>
@@ -5642,7 +5646,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C29" t="s">
         <v>135</v>
@@ -5657,7 +5661,7 @@
         <v>307</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>221</v>
@@ -5671,7 +5675,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C30" t="s">
         <v>142</v>
@@ -5683,10 +5687,10 @@
         <v>184</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>242</v>
@@ -5700,7 +5704,7 @@
         <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
@@ -5709,13 +5713,13 @@
         <v>7</v>
       </c>
       <c r="E31" t="s">
+        <v>366</v>
+      </c>
+      <c r="F31" t="s">
         <v>367</v>
       </c>
-      <c r="F31" t="s">
-        <v>368</v>
-      </c>
       <c r="G31" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H31" s="14" t="s">
         <v>259</v>
@@ -5729,25 +5733,25 @@
         <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D32" t="s">
         <v>111</v>
       </c>
       <c r="E32" t="s">
+        <v>434</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="G32" s="10" t="s">
+      <c r="H32" t="s">
         <v>436</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>437</v>
-      </c>
-      <c r="I32" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -5755,7 +5759,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D33" t="s">
         <v>167</v>
@@ -5781,7 +5785,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D34" t="s">
         <v>133</v>
@@ -5790,7 +5794,7 @@
         <v>132</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>134</v>
@@ -5807,7 +5811,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C35" t="s">
         <v>147</v>
@@ -5836,7 +5840,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -5862,7 +5866,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C37" t="s">
         <v>119</v>
@@ -5891,7 +5895,7 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C38" t="s">
         <v>243</v>
@@ -5920,7 +5924,7 @@
         <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C39" t="s">
         <v>231</v>
@@ -5949,7 +5953,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C40" t="s">
         <v>350</v>
@@ -5978,7 +5982,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C41" t="s">
         <v>243</v>
@@ -6004,7 +6008,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D42">
         <v>10</v>
@@ -6030,7 +6034,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C43" t="s">
         <v>125</v>
@@ -6059,7 +6063,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D44" t="s">
         <v>277</v>
@@ -6068,7 +6072,7 @@
         <v>200</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>123</v>
@@ -6085,7 +6089,7 @@
         <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C45" t="s">
         <v>142</v>
@@ -6114,7 +6118,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D46">
         <v>8</v>
@@ -6140,7 +6144,7 @@
         <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D47">
         <v>20</v>
@@ -6166,7 +6170,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C48" t="s">
         <v>287</v>
@@ -6195,7 +6199,7 @@
         <v>32</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -6221,7 +6225,7 @@
         <v>35</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C50" t="s">
         <v>243</v>
@@ -6250,7 +6254,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D51">
         <v>20</v>
@@ -6276,7 +6280,7 @@
         <v>36</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C52" t="s">
         <v>243</v>
@@ -6305,7 +6309,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D53">
         <v>10</v>
@@ -6331,7 +6335,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C54" t="s">
         <v>267</v>
@@ -6360,7 +6364,7 @@
         <v>41</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C55" t="s">
         <v>275</v>
@@ -6389,7 +6393,7 @@
         <v>42</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D56" t="s">
         <v>277</v>
@@ -6415,7 +6419,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D57" t="s">
         <v>274</v>
@@ -6441,7 +6445,7 @@
         <v>46</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D58" t="s">
         <v>288</v>
@@ -6467,7 +6471,7 @@
         <v>47</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D59" t="s">
         <v>296</v>
@@ -6493,7 +6497,7 @@
         <v>49</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D60" t="s">
         <v>269</v>
@@ -6505,7 +6509,7 @@
         <v>357</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H60" t="s">
         <v>271</v>
@@ -6519,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C61" t="s">
         <v>85</v>
@@ -6531,7 +6535,7 @@
         <v>79</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>84</v>
@@ -6548,7 +6552,7 @@
         <v>52</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E62" t="s">
         <v>340</v>
@@ -6560,17 +6564,17 @@
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I65" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I66" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I67" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.25">
@@ -6578,7 +6582,7 @@
         <v>116</v>
       </c>
       <c r="I68" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.25">
@@ -6586,7 +6590,7 @@
         <v>64</v>
       </c>
       <c r="I69" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.25">
@@ -6594,7 +6598,7 @@
         <v>248</v>
       </c>
       <c r="I70" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.25">
@@ -6602,7 +6606,7 @@
         <v>245</v>
       </c>
       <c r="I71" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.25">
@@ -6684,140 +6688,140 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2" t="s">
         <v>376</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>377</v>
-      </c>
-      <c r="C2" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" t="s">
         <v>379</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>380</v>
-      </c>
-      <c r="C3" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>447</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="L11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D12" s="19">
         <v>8</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -6825,31 +6829,31 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
+        <v>513</v>
+      </c>
+      <c r="C13" t="s">
+        <v>439</v>
+      </c>
+      <c r="D13" t="s">
+        <v>528</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H13" t="s">
+        <v>451</v>
+      </c>
+      <c r="I13" t="s">
+        <v>441</v>
+      </c>
+      <c r="J13" t="s">
         <v>440</v>
       </c>
-      <c r="D13" t="s">
-        <v>529</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>564</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>515</v>
-      </c>
-      <c r="H13" t="s">
-        <v>452</v>
-      </c>
-      <c r="I13" t="s">
-        <v>442</v>
-      </c>
-      <c r="J13" t="s">
-        <v>441</v>
-      </c>
       <c r="L13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -6857,28 +6861,28 @@
         <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C14" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D14" s="19">
         <v>26</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -6886,10 +6890,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D15" s="19">
         <v>8</v>
@@ -6902,10 +6906,10 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M15" s="20"/>
       <c r="O15" s="20"/>
@@ -6918,13 +6922,13 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C16" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>231</v>
@@ -6933,10 +6937,10 @@
         <v>7</v>
       </c>
       <c r="I16" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -6944,16 +6948,16 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D17" s="19">
         <v>7</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>7</v>
@@ -6962,7 +6966,7 @@
         <v>7</v>
       </c>
       <c r="J17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -6970,28 +6974,28 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D18" s="19">
         <v>20</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F18" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -6999,28 +7003,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D19" s="26">
         <v>20</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J19" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -7028,28 +7032,28 @@
         <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D20" s="19">
         <v>7</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F20" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -7057,10 +7061,10 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D21" s="19">
         <v>10</v>
@@ -7072,10 +7076,10 @@
         <v>7</v>
       </c>
       <c r="J21" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -7083,25 +7087,25 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C22" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L22" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -7112,27 +7116,27 @@
         <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D25">
         <v>8</v>
@@ -7141,29 +7145,29 @@
         <v>7</v>
       </c>
       <c r="L25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D26" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>7</v>
@@ -7171,7 +7175,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C28" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D28" s="19">
         <v>24</v>
@@ -7180,26 +7184,26 @@
         <v>7</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D30">
         <v>60</v>
@@ -7208,21 +7212,21 @@
         <v>7</v>
       </c>
       <c r="L30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D31" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -7230,7 +7234,7 @@
         <v>7</v>
       </c>
       <c r="L32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -7238,12 +7242,12 @@
         <v>7</v>
       </c>
       <c r="L33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>7</v>
@@ -7251,46 +7255,46 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L35" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L36" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L37" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -7299,29 +7303,29 @@
         <v>7</v>
       </c>
       <c r="L39" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L40" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -7332,7 +7336,7 @@
         <v>7</v>
       </c>
       <c r="L42" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -7359,12 +7363,12 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -7374,12 +7378,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
@@ -7394,12 +7398,12 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -7437,38 +7441,38 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>447</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P3" s="30" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Q3" s="30" t="s">
         <v>71</v>
@@ -7479,22 +7483,22 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D4" s="19">
         <v>24</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P4" s="31">
         <v>24</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -7502,10 +7506,10 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D5" s="19">
         <v>8</v>
@@ -7525,22 +7529,22 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q6" s="31" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -7548,48 +7552,48 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D7" s="19">
         <v>7</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="P7" s="32">
         <v>7</v>
       </c>
       <c r="Q7" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D8" s="31">
         <v>8</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P8" s="31">
         <v>8</v>
       </c>
       <c r="Q8" s="31" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -7597,22 +7601,22 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="P9" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q9" s="32" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -7620,25 +7624,25 @@
         <v>48</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>231</v>
       </c>
       <c r="H10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="P10" s="31" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Q10" s="31" t="s">
         <v>231</v>
@@ -7649,19 +7653,19 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D11" s="19">
         <v>7</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="P11" s="32">
         <v>10</v>
@@ -7675,10 +7679,10 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D12" s="19">
         <v>10</v>
@@ -7687,16 +7691,16 @@
         <v>208</v>
       </c>
       <c r="H12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I12" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P12" s="31">
         <v>7</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -7704,25 +7708,25 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D13" s="19">
         <v>20</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="P13" s="32">
         <v>20</v>
       </c>
       <c r="Q13" s="32" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -7730,44 +7734,44 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C14" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D14" s="26">
         <v>20</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F14" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H14" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I14" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P14" s="33">
         <v>20</v>
       </c>
       <c r="Q14" s="33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -7776,54 +7780,54 @@
         <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D18" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I18">
         <f>I17*0.5</f>
         <v>17</v>
       </c>
       <c r="J18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C20" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D20" s="19">
         <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D22">
         <v>60</v>
@@ -7831,13 +7835,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D23" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I23" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -7845,7 +7849,7 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7853,13 +7857,13 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I25">
         <v>5</v>
       </c>
       <c r="J25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -7867,14 +7871,14 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I26">
         <f>I24*4+I25*3</f>
         <v>35</v>
       </c>
       <c r="J26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -7882,7 +7886,7 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -7891,42 +7895,42 @@
         <v>60</v>
       </c>
       <c r="J28" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I29">
         <f>I25*3*1</f>
         <v>15</v>
       </c>
       <c r="J29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B30" t="s">
+        <v>595</v>
+      </c>
+      <c r="C30" t="s">
         <v>596</v>
-      </c>
-      <c r="C30" t="s">
-        <v>597</v>
       </c>
       <c r="I30">
         <f>I29+I28</f>
         <v>75</v>
       </c>
       <c r="J30" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B31">
         <v>170</v>
@@ -7936,12 +7940,12 @@
         <v>34</v>
       </c>
       <c r="J31" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B32">
         <v>190</v>
@@ -7953,7 +7957,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B33">
         <v>270</v>
@@ -7963,20 +7967,20 @@
         <v>54</v>
       </c>
       <c r="I33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -7984,12 +7988,12 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -7998,7 +8002,7 @@
         <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -8007,20 +8011,20 @@
         <v>42.5</v>
       </c>
       <c r="B41" t="s">
+        <v>417</v>
+      </c>
+      <c r="C41" t="s">
         <v>418</v>
-      </c>
-      <c r="C41" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -8028,7 +8032,7 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -8036,7 +8040,7 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -8045,7 +8049,7 @@
         <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -8054,7 +8058,7 @@
         <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -8063,7 +8067,7 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -8072,27 +8076,27 @@
         <v>180</v>
       </c>
       <c r="B52" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -8126,150 +8130,150 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>590</v>
+      </c>
+      <c r="B9" t="s">
         <v>591</v>
-      </c>
-      <c r="B9" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B10" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B11" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B13" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B16" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>593</v>
+      </c>
+      <c r="B18" t="s">
         <v>594</v>
-      </c>
-      <c r="B18" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B19" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B21" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B22" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -8289,47 +8293,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
printout and added some work acceptions
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="676">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2307,39 +2307,6 @@
   </si>
   <si>
     <t>Text Customization</t>
-  </si>
-  <si>
-    <t>* Lexicon for similar related words
-* There are good lexicons
-* there are machine learning/AI natural language processing - Brian to look into
-*Search for subword in sentence to accept if right things in there as long as doesn't interprut the wrong action
-* Worse thing in a game as a player is to know what to do but not how to do it 
-* Have a whole user input module that deciphers input
-From Written Work
-*1. Parsing system where verb is first and then searches for noun based on context of surroundings
-E.g. attack
-Some verbs like "pick" are contextual based on selected noun, item, interact, person so will have to test.
-*2. Parsing looking for verb and noun in sentence based on context of surrounding
-* Be able to use any part (space delimited) of the name if an item, interactable, or enemy in the spellchecker and acceptor as long as it only closely matches one
-*Spell check will have to look at the important words and try to match based on context of surroundings (all entities in that locations) 
-*Either way it will boil down to context of the game. There are only so many functions that words can go into. NO NEW FUNCTIONS WILL BE MADE BASED ON PARSER
-*WILL Need testers for parser AND it will boil down
-*Can Break this down into time with lots of time to developed and test
-*Multiple rules signs with different aspects
-When you first load in it explains accepted words
-Movement infront of JHE
-Talking and Reading (read everything) with Kenrick (spawns things)
-Inspecting things and talking to people (quests) in BSB field with msp430 and trash can and also Mitch with his cell phone or keys or Wallet
-Explain how talking or completing quest can unlock/spawn people. There are different ways to get what you want, sometimes you can talk, sometimes all it takes is getting something, but other times you need to take it by force
-Attacking things in JHE field with low-level person like a dummy or something 
-shortcuts and settings
-On notes if they are added
-Feedback, bugs, offensive contents and updates! 
-Overview of game functions
-People have to exit in order for the game to save game (have to explain this somehow in the tutorial)
-• Nice to have is after you read the sign and copy it down in your notes it disappears
-• You can examine people (just says that's Dr Summerville, it's rude to state"), places (gives you lore and looks around again), and things (Items and injectables)
-• first message explains parsing and inspecting and says "to learn more, look at that tutorial sign"</t>
   </si>
   <si>
     <t>* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
@@ -2451,6 +2418,30 @@
     <t>23 - 3.5 Writing Auto Descriptions and fixing descriptions</t>
   </si>
   <si>
+    <t>24 - 1.25 Finish Basic version of auto surroundings, documented, and started playing with compiler</t>
+  </si>
+  <si>
+    <t>* Overwriting old instal to update would be nice.
+* Settings being weird are probably due to DEV MODE option (maybe just have dev mode file with key or SOMETHING IDK)
+Maybe have Devmode if you run it with a -DEBUG or something in the command line. Not sure how to do those but would like to.
+*remove the build folder (or see how little it can operate off of), rename the dist folder, and remove the "-amd64" possibly from the file name
+Done:
+*ADDED Make so it takes files/folders automatically when put in includefiles
+How to include files
+https://stackoverflow.com/questions/2553886/how-can-i-bundle-other-files-when-using-cx-freeze
+Needs relative file locations!
+*ADDED Icon populates automatically and Desktop Icon Automatically (with proper working directory)</t>
+  </si>
+  <si>
+    <t>27 - 2 hr Debuging compilier working directory, trying to get shortcut icon setup, commenting code</t>
+  </si>
+  <si>
+    <t>26 - 1.25 Getting Compilier to go more</t>
+  </si>
+  <si>
+    <t>540/9 hr</t>
+  </si>
+  <si>
     <t>* Improved surroundings
 The description can be turned into a more in-depth first time description of the place, item, with more detail
 Look, or look around gives the long description
@@ -2480,7 +2471,7 @@
 The name is surounded by ~ ~ and all captalized when printed through MAP.search
 No delimters (the), prepositions (in, outside), or qualifying words (very)
 Use direction with reference to areas
- ex)       Front of Hatch. Behind Art Museum. JHE Lobby
+ ex)       Behind Hatch. Infront of Art Museum. JHE Lobby
  NOT example) Outside Hatch. Outside Art Museum. Inside JHE
  exceptions) THE Phoniex (where it's a name)
 Just very basic name of the word that you would want to read quickly
@@ -2515,22 +2506,42 @@
 *ADDED Look around now accepted to give search, remember give the lore, wait+sit+sleep to pass time, and die to exit the game</t>
   </si>
   <si>
-    <t>24 - 1.25 Finish Basic version of auto surroundings, documented, and started playing with compiler</t>
-  </si>
-  <si>
-    <t>* Get the shortcut to not make cache and also for thing to thing
-* does code checks print out
-* Overwriting old instal to update would be nice.
-*remove the build folder and rename the dist folder
+    <t>28 - 1.5 hr  Cleaned up the printout a bit, made it so you can now do "pick up" (item), "use (item)", "give (item)" items in the NLP</t>
+  </si>
+  <si>
+    <t>* Lexicon for similar related words
+* There are good lexicons
+* there are machine learning/AI natural language processing - Brian to look into
+*Search for subword in sentence to accept if right things in there as long as doesn't interprut the wrong action
+* Worse thing in a game as a player is to know what to do but not how to do it 
+* Have a whole user input module that deciphers input
+From Written Work
+*1. Parsing system where verb is first and then searches for noun based on context of surroundings
+E.g. attack
+Some verbs like "pick" are contextual based on selected noun, item, interact, person so will have to test.
+*2. Parsing looking for verb and noun in sentence based on context of surrounding
+* Be able to use any part (space delimited) of the name if an item, interactable, or enemy in the spellchecker and acceptor as long as it only closely matches one
+*Spell check will have to look at the important words and try to match based on context of surroundings (all entities in that locations) 
+*Either way it will boil down to context of the game. There are only so many functions that words can go into. NO NEW FUNCTIONS WILL BE MADE BASED ON PARSER
+*WILL Need testers for parser AND it will boil down
+*Can Break this down into time with lots of time to developed and test
+*Multiple rules signs with different aspects
+When you first load in it explains accepted words
+Movement infront of JHE
+Talking and Reading (read everything) with Kenrick (spawns things)
+Inspecting things and talking to people (quests) in BSB field with msp430 and trash can and also Mitch with his cell phone or keys or Wallet
+Explain how talking or completing quest can unlock/spawn people. There are different ways to get what you want, sometimes you can talk, sometimes all it takes is getting something, but other times you need to take it by force
+Attacking things in JHE field with low-level person like a dummy or something 
+shortcuts and settings
+On notes if they are added
+Feedback, bugs, offensive contents and updates! 
+Overview of game functions
+People have to exit in order for the game to save game (have to explain this somehow in the tutorial)
+• Nice to have is after you read the sign and copy it down in your notes it disappears
+• You can examine people (just says that's Dr Summerville, it's rude to state"), places (gives you lore and looks around again), and things (Items and injectables)
+• first message explains parsing and inspecting and says "to learn more, look at that tutorial sign"
 Done:
-*ADDED Make so it takes files/folders automatically when put in includefiles
-How to include files
-https://stackoverflow.com/questions/2553886/how-can-i-bundle-other-files-when-using-cx-freeze
-Needs relative file locations!
-*ADDED Icon populates automatically and Desktop Icon Automatically</t>
-  </si>
-  <si>
-    <t>26 - 1.15 Getting Compilier to go more</t>
+ADDED You can now do "pick up" (item), "use (item)" which uses it on any relavant interactables, "give (item)" which gives it to any relavant NPCs around</t>
   </si>
 </sst>
 </file>
@@ -3259,7 +3270,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,16 +3492,16 @@
         <v>648</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F14" t="s">
+        <v>661</v>
+      </c>
+      <c r="G14" t="s">
         <v>662</v>
       </c>
-      <c r="G14" t="s">
-        <v>663</v>
-      </c>
       <c r="H14" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I14" t="s">
         <v>548</v>
@@ -3504,7 +3515,7 @@
         <v>616</v>
       </c>
       <c r="C15" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D15" t="s">
         <v>618</v>
@@ -3521,30 +3532,33 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B16" t="s">
         <v>624</v>
       </c>
       <c r="C16" t="s">
+        <v>667</v>
+      </c>
+      <c r="D16" t="s">
         <v>668</v>
-      </c>
-      <c r="D16" t="s">
-        <v>670</v>
       </c>
       <c r="E16" t="s">
         <v>627</v>
       </c>
       <c r="F16" t="s">
+        <v>671</v>
+      </c>
+      <c r="G16" t="s">
+        <v>670</v>
+      </c>
+      <c r="H16" t="s">
         <v>672</v>
-      </c>
-      <c r="G16" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>641</v>
+        <v>674</v>
       </c>
       <c r="B17" t="s">
         <v>630</v>
@@ -3624,13 +3638,13 @@
         <v>543</v>
       </c>
       <c r="C29" t="s">
+        <v>658</v>
+      </c>
+      <c r="D29" t="s">
         <v>659</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>660</v>
-      </c>
-      <c r="E29" t="s">
-        <v>661</v>
       </c>
       <c r="F29" t="s">
         <v>546</v>
@@ -4830,8 +4844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4958,7 +4972,7 @@
         <v>148</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>500</v>
@@ -5041,7 +5055,7 @@
         <v>169</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>500</v>
@@ -5085,7 +5099,7 @@
         <v>208</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>500</v>
@@ -5248,7 +5262,7 @@
         <v>465</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>500</v>
@@ -5274,7 +5288,7 @@
         <v>563</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>654</v>
+        <v>675</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>500</v>
@@ -6535,7 +6549,7 @@
         <v>79</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>84</v>
@@ -7886,7 +7900,7 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added colours, parser functions, and changed RNG down
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="679">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2509,12 +2509,14 @@
     <t>28 - 1.5 hr  Cleaned up the printout a bit, made it so you can now do "pick up" (item), "use (item)", "give (item)" items in the NLP</t>
   </si>
   <si>
-    <t>* Lexicon for similar related words
-* There are good lexicons
-* there are machine learning/AI natural language processing - Brian to look into
-*Search for subword in sentence to accept if right things in there as long as doesn't interprut the wrong action
+    <t>29 - 4.25 hr researching parsers more, implementing help function/better tutorial, doing parser shortcuts, designing parser subword search</t>
+  </si>
+  <si>
+    <t>Nice to have
+*INFOCOM style parser, Search for subword in sentence to accept if right things in there as long as doesn't interprut the wrong action
+This includes verb and noun subsearch, accepting multile things with THEN AND
+*Tutorial in the startup menu to teach or tutorial signs
 * Worse thing in a game as a player is to know what to do but not how to do it 
-* Have a whole user input module that deciphers input
 From Written Work
 *1. Parsing system where verb is first and then searches for noun based on context of surroundings
 E.g. attack
@@ -2525,6 +2527,7 @@
 *Either way it will boil down to context of the game. There are only so many functions that words can go into. NO NEW FUNCTIONS WILL BE MADE BASED ON PARSER
 *WILL Need testers for parser AND it will boil down
 *Can Break this down into time with lots of time to developed and test
+Tutorial
 *Multiple rules signs with different aspects
 When you first load in it explains accepted words
 Movement infront of JHE
@@ -2538,10 +2541,21 @@
 Overview of game functions
 People have to exit in order for the game to save game (have to explain this somehow in the tutorial)
 • Nice to have is after you read the sign and copy it down in your notes it disappears
-• You can examine people (just says that's Dr Summerville, it's rude to state"), places (gives you lore and looks around again), and things (Items and injectables)
-• first message explains parsing and inspecting and says "to learn more, look at that tutorial sign"
 Done:
-ADDED You can now do "pick up" (item), "use (item)" which uses it on any relavant interactables, "give (item)" which gives it to any relavant NPCs around</t>
+ADDED You can now do "pick up" (item), "use (item)" which uses it on any relavant interactables, "give (item)" which gives it to any relavant NPCs around
+CHANGED Made TextParser.py module for all the text parsing code
+ADDED Help function which displays help and shortcuts to objects
+ADDED Verb shortcuts for parsing
+ADDED Shorkeys which are (unfortunately dynamic) numbers which you can use to pick up stuff (1-4 reserved for inventory items)
+CHANGED Tutorial Sign now disapears
+ADDED More juicy responses with examining someone gives "It's rude to stare", trying to eat something gives "You try to eat them but they pull away"
+CHANGED Start text and response text in situations to try to make it more immersive to the storyline</t>
+  </si>
+  <si>
+    <t>30 - 2 hr Fixing shortkey parser, working on the word subsearch</t>
+  </si>
+  <si>
+    <t>31 - 2 hr crafting colours, clearscreen, prinout, and getting feedback from the hommies</t>
   </si>
 </sst>
 </file>
@@ -2679,7 +2693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2741,6 +2755,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3270,7 +3287,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3561,13 +3578,13 @@
         <v>674</v>
       </c>
       <c r="B17" t="s">
-        <v>630</v>
+        <v>675</v>
       </c>
       <c r="C17" t="s">
-        <v>642</v>
+        <v>677</v>
       </c>
       <c r="D17" t="s">
-        <v>631</v>
+        <v>678</v>
       </c>
       <c r="E17" t="s">
         <v>632</v>
@@ -3814,8 +3831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="F41" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:K7"/>
+    <sheetView topLeftCell="F29" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5274,7 +5291,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>56</v>
       </c>
@@ -5287,8 +5304,8 @@
       <c r="E15" t="s">
         <v>563</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>675</v>
+      <c r="F15" s="36" t="s">
+        <v>676</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>500</v>

</xml_diff>

<commit_message>
Adding more juicy responses, debugging parser more, and documentating parser
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -22,7 +22,7 @@
     <sheet name="Habit Diagram" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alpha 0.30 Feature Lock'!$A$4:$I$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alpha 0.30 Feature Lock'!$A$4:$I$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Feedback!$A$1:$F$50</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="684">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2512,21 +2512,20 @@
     <t>29 - 4.25 hr researching parsers more, implementing help function/better tutorial, doing parser shortcuts, designing parser subword search</t>
   </si>
   <si>
+    <t>30 - 2 hr Fixing shortkey parser, working on the word subsearch</t>
+  </si>
+  <si>
+    <t>31 - 2 hr crafting colours, clearscreen, prinout, and getting feedback from the hommies</t>
+  </si>
+  <si>
+    <t>NOV 1 - 1 hr Finishing subword noun parser, writing documentation</t>
+  </si>
+  <si>
     <t>Nice to have
 *INFOCOM style parser, Search for subword in sentence to accept if right things in there as long as doesn't interprut the wrong action
 This includes verb and noun subsearch, accepting multile things with THEN AND
 *Tutorial in the startup menu to teach or tutorial signs
 * Worse thing in a game as a player is to know what to do but not how to do it 
-From Written Work
-*1. Parsing system where verb is first and then searches for noun based on context of surroundings
-E.g. attack
-Some verbs like "pick" are contextual based on selected noun, item, interact, person so will have to test.
-*2. Parsing looking for verb and noun in sentence based on context of surrounding
-* Be able to use any part (space delimited) of the name if an item, interactable, or enemy in the spellchecker and acceptor as long as it only closely matches one
-*Spell check will have to look at the important words and try to match based on context of surroundings (all entities in that locations) 
-*Either way it will boil down to context of the game. There are only so many functions that words can go into. NO NEW FUNCTIONS WILL BE MADE BASED ON PARSER
-*WILL Need testers for parser AND it will boil down
-*Can Break this down into time with lots of time to developed and test
 Tutorial
 *Multiple rules signs with different aspects
 When you first load in it explains accepted words
@@ -2544,18 +2543,44 @@
 Done:
 ADDED You can now do "pick up" (item), "use (item)" which uses it on any relavant interactables, "give (item)" which gives it to any relavant NPCs around
 CHANGED Made TextParser.py module for all the text parsing code
-ADDED Help function which displays help and shortcuts to objects
-ADDED Verb shortcuts for parsing
-ADDED Shorkeys which are (unfortunately dynamic) numbers which you can use to pick up stuff (1-4 reserved for inventory items)
+ADDED 'Hel'p verb which displays help and a 'shortcuts' which displays list of shortcuts
+ADDED Shorkeys which are (unfortunately dynamic) numbers which you can use to pick up stuff in order it appears (1-4 reserved for inventory items)
 CHANGED Tutorial Sign now disapears
-ADDED More juicy responses with examining someone gives "It's rude to stare", trying to eat something gives "You try to eat them but they pull away"
-CHANGED Start text and response text in situations to try to make it more immersive to the storyline</t>
-  </si>
-  <si>
-    <t>30 - 2 hr Fixing shortkey parser, working on the word subsearch</t>
-  </si>
-  <si>
-    <t>31 - 2 hr crafting colours, clearscreen, prinout, and getting feedback from the hommies</t>
+ADDED More juicy responses with examining someone gives "It's rude to stare", trying to eat someone gives "You try to eat them but they pull away", trying to equip someone says "You attempt to pick up  __ and now you're both really uncomfortable."
+CHANGED Start text and response text in situations to try to make it more immersive to the storyline
+ADDED Bassically a noun subword search so you can type pretty much any amount of a word and will search. Highly unoptimized but hopefully won't run into problems</t>
+  </si>
+  <si>
+    <t>Polish 1</t>
+  </si>
+  <si>
+    <t>* Add accepting for each senario
+go _
+ &lt;objects&gt;, /interacts/, and [people]
+equipt _
+ &lt;objects&gt;, /interacts/, and [people]
+drop _
+ &lt;objects&gt;, /interacts/, and [people]
+inspect _
+ &lt;objects&gt;, /interacts/, and [people]
+eat _
+ &lt;objects&gt;, /interacts/, and [people]
+use _
+ &lt;objects&gt;, /interacts/, and [people]
+talk _
+ &lt;objects&gt;, /interacts/, and [people]
+give _
+ &lt;objects&gt;, /interacts/, and [people]
+attack _
+ &lt;objects&gt;, /interacts/, and [people]
+* Implement feedback
+*Playtests?</t>
+  </si>
+  <si>
+    <t>EPTA is at 4600 Lines of code!</t>
+  </si>
+  <si>
+    <t>2 - 2 hr Adding more juicy responses, debugging parser more, and documentating parser</t>
   </si>
 </sst>
 </file>
@@ -2693,7 +2718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2755,9 +2780,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2963,8 +2985,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I62" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A4:I62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I63" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A4:I63"/>
   <sortState ref="A5:I62">
     <sortCondition ref="G4:G62"/>
   </sortState>
@@ -3286,8 +3308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3581,19 +3603,22 @@
         <v>675</v>
       </c>
       <c r="C17" t="s">
+        <v>676</v>
+      </c>
+      <c r="D17" t="s">
         <v>677</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>678</v>
       </c>
-      <c r="E17" t="s">
-        <v>632</v>
-      </c>
       <c r="F17" t="s">
-        <v>633</v>
+        <v>683</v>
       </c>
       <c r="G17" t="s">
         <v>634</v>
+      </c>
+      <c r="I17" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3831,7 +3856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="F29" workbookViewId="0">
+    <sheetView topLeftCell="F44" workbookViewId="0">
       <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
@@ -4859,10 +4884,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5291,7 +5316,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>56</v>
       </c>
@@ -5304,8 +5329,8 @@
       <c r="E15" t="s">
         <v>563</v>
       </c>
-      <c r="F15" s="36" t="s">
-        <v>676</v>
+      <c r="F15" s="14" t="s">
+        <v>679</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>500</v>
@@ -5346,1340 +5371,1355 @@
         <v>647</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>58</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="E17" t="s">
+        <v>680</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>681</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23">
         <v>18</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B18" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C18" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D18" s="23">
         <v>20</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E18" s="23" t="s">
         <v>522</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F18" s="24" t="s">
         <v>562</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G18" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="H18" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I18" s="23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+    <row r="19" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
         <v>50</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B19" s="27" t="s">
         <v>515</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C19" s="26" t="s">
         <v>369</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D19" s="26">
         <v>7</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E19" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F19" s="29" t="s">
         <v>533</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G19" s="28" t="s">
         <v>502</v>
       </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="D19">
-        <v>1.5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="H19" t="s">
-        <v>86</v>
-      </c>
-      <c r="I19" t="s">
-        <v>87</v>
-      </c>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C20" t="s">
-        <v>102</v>
-      </c>
       <c r="D20">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="I20" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>355</v>
+        <v>99</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>514</v>
-      </c>
-      <c r="D22" t="s">
-        <v>364</v>
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>355</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H22" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I22" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="C23" t="s">
-        <v>112</v>
-      </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>364</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>530</v>
+        <v>361</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="D24">
-        <v>9</v>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>111</v>
       </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>58</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>469</v>
+        <v>530</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H24" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="I24" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="D25" t="s">
-        <v>410</v>
+      <c r="D25">
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>506</v>
+        <v>469</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>514</v>
+      </c>
+      <c r="D26" t="s">
+        <v>410</v>
+      </c>
+      <c r="E26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="H26" t="s">
         <v>141</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="26">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="26">
         <v>13</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B27" s="34" t="s">
         <v>514</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C27" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D27" s="26">
         <v>10</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E27" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F27" s="29" t="s">
         <v>468</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G27" s="28" t="s">
         <v>378</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="H27" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="I26" s="26" t="s">
+      <c r="I27" s="26" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>14</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>514</v>
-      </c>
-      <c r="C27" t="s">
-        <v>143</v>
-      </c>
-      <c r="D27">
-        <v>10</v>
-      </c>
-      <c r="E27" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="H27" t="s">
-        <v>144</v>
-      </c>
-      <c r="I27" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>19</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>515</v>
+        <v>14</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>514</v>
+      </c>
+      <c r="C28" t="s">
+        <v>143</v>
       </c>
       <c r="D28">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>305</v>
+        <v>360</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H28" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="I28" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>26</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>514</v>
-      </c>
-      <c r="C29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D29" t="s">
-        <v>220</v>
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="H29" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>222</v>
+      <c r="H29" t="s">
+        <v>162</v>
+      </c>
+      <c r="I29" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>34</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>515</v>
+        <v>26</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>514</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30">
-        <v>6</v>
+        <v>135</v>
+      </c>
+      <c r="D30" t="s">
+        <v>220</v>
       </c>
       <c r="E30" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>454</v>
+        <v>307</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>114</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>515</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>366</v>
-      </c>
-      <c r="F31" t="s">
-        <v>367</v>
+        <v>184</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>454</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>378</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>260</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D32" t="s">
-        <v>111</v>
+        <v>515</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>434</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>438</v>
+        <v>366</v>
+      </c>
+      <c r="F32" t="s">
+        <v>367</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="H32" t="s">
-        <v>436</v>
-      </c>
-      <c r="I32" t="s">
-        <v>437</v>
+        <v>378</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>517</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="E33" t="s">
-        <v>164</v>
-      </c>
-      <c r="F33" t="s">
-        <v>306</v>
+        <v>434</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>438</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="H33" t="s">
-        <v>166</v>
+        <v>436</v>
       </c>
       <c r="I33" t="s">
-        <v>165</v>
+        <v>437</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>517</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="E34" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>470</v>
+        <v>164</v>
+      </c>
+      <c r="F34" t="s">
+        <v>306</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="H34" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="I34" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C35" t="s">
-        <v>147</v>
-      </c>
-      <c r="D35">
-        <v>6</v>
+      <c r="D35" t="s">
+        <v>133</v>
       </c>
       <c r="E35" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>359</v>
+        <v>470</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>134</v>
       </c>
       <c r="H35" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I35" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="C36" t="s">
+        <v>147</v>
+      </c>
       <c r="D36">
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>177</v>
-      </c>
-      <c r="F36" t="s">
-        <v>310</v>
+        <v>145</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>359</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="H36" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>114</v>
+      <c r="H36" t="s">
+        <v>146</v>
+      </c>
+      <c r="I36" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C37" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" t="s">
-        <v>118</v>
+      <c r="D37">
+        <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>117</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>303</v>
+        <v>177</v>
+      </c>
+      <c r="F37" t="s">
+        <v>310</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H37" t="s">
-        <v>122</v>
-      </c>
-      <c r="I37" t="s">
-        <v>128</v>
+        <v>134</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>517</v>
       </c>
       <c r="C38" t="s">
-        <v>243</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>214</v>
+        <v>118</v>
       </c>
       <c r="E38" t="s">
-        <v>206</v>
+        <v>117</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="G38" s="10" t="s">
         <v>121</v>
       </c>
       <c r="H38" t="s">
-        <v>213</v>
+        <v>122</v>
       </c>
       <c r="I38" t="s">
-        <v>212</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>517</v>
       </c>
       <c r="C39" t="s">
-        <v>231</v>
-      </c>
-      <c r="D39">
-        <v>16</v>
+        <v>243</v>
+      </c>
+      <c r="D39" t="s">
+        <v>214</v>
       </c>
       <c r="E39" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>233</v>
+        <v>121</v>
+      </c>
+      <c r="H39" t="s">
+        <v>213</v>
+      </c>
+      <c r="I39" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>517</v>
       </c>
       <c r="C40" t="s">
-        <v>350</v>
-      </c>
-      <c r="D40" t="s">
-        <v>111</v>
+        <v>231</v>
+      </c>
+      <c r="D40">
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="H40" t="s">
-        <v>157</v>
-      </c>
-      <c r="I40" t="s">
-        <v>158</v>
+        <v>230</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>517</v>
       </c>
       <c r="C41" t="s">
-        <v>243</v>
+        <v>350</v>
+      </c>
+      <c r="D41" t="s">
+        <v>111</v>
       </c>
       <c r="E41" t="s">
-        <v>350</v>
+        <v>155</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="G41" t="s">
+        <v>353</v>
+      </c>
+      <c r="G41" s="10" t="s">
         <v>156</v>
       </c>
       <c r="H41" t="s">
-        <v>352</v>
+        <v>157</v>
       </c>
       <c r="I41" t="s">
-        <v>351</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="D42">
-        <v>10</v>
+      <c r="C42" t="s">
+        <v>243</v>
       </c>
       <c r="E42" t="s">
-        <v>187</v>
+        <v>350</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="H42" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>257</v>
+        <v>354</v>
+      </c>
+      <c r="G42" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" t="s">
+        <v>352</v>
+      </c>
+      <c r="I42" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" t="s">
-        <v>118</v>
+      <c r="D43">
+        <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>124</v>
-      </c>
-      <c r="F43" t="s">
-        <v>304</v>
+        <v>187</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>314</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="H43" t="s">
-        <v>126</v>
-      </c>
-      <c r="I43" t="s">
-        <v>127</v>
+        <v>255</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="C44" t="s">
+        <v>125</v>
+      </c>
       <c r="D44" t="s">
-        <v>277</v>
+        <v>118</v>
       </c>
       <c r="E44" t="s">
-        <v>200</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>565</v>
+        <v>124</v>
+      </c>
+      <c r="F44" t="s">
+        <v>304</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H44" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>283</v>
+      <c r="H44" t="s">
+        <v>126</v>
+      </c>
+      <c r="I44" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C45" t="s">
-        <v>142</v>
-      </c>
-      <c r="D45">
-        <v>10</v>
+      <c r="D45" t="s">
+        <v>277</v>
       </c>
       <c r="E45" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>309</v>
+        <v>565</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="H45" t="s">
-        <v>216</v>
-      </c>
-      <c r="I45" t="s">
-        <v>217</v>
+        <v>123</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="C46" t="s">
+        <v>142</v>
+      </c>
       <c r="D46">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="H46" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="I46" s="14" t="s">
-        <v>224</v>
+      <c r="H46" t="s">
+        <v>216</v>
+      </c>
+      <c r="I46" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>517</v>
       </c>
       <c r="D47">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>302</v>
+        <v>202</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C48" t="s">
-        <v>287</v>
-      </c>
-      <c r="D48" t="s">
-        <v>284</v>
+      <c r="D48">
+        <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>201</v>
+        <v>302</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>234</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>285</v>
+        <v>235</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="D49">
-        <v>10</v>
+      <c r="C49" t="s">
+        <v>287</v>
+      </c>
+      <c r="D49" t="s">
+        <v>284</v>
       </c>
       <c r="E49" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>239</v>
+        <v>285</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>237</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C50" t="s">
-        <v>243</v>
-      </c>
       <c r="D50">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>313</v>
+        <v>349</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="C51" t="s">
+        <v>243</v>
+      </c>
       <c r="D51">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>292</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C52" t="s">
-        <v>243</v>
-      </c>
       <c r="D52">
         <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>254</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="C53" t="s">
+        <v>243</v>
+      </c>
       <c r="D53">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E53" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>315</v>
+        <v>344</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>252</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C54" t="s">
-        <v>267</v>
-      </c>
-      <c r="D54" t="s">
-        <v>266</v>
+      <c r="D54">
+        <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>252</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>154</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>517</v>
       </c>
       <c r="C55" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D55" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="E55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>273</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="C56" t="s">
+        <v>275</v>
+      </c>
       <c r="D56" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>261</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>517</v>
       </c>
       <c r="D57" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>517</v>
       </c>
       <c r="D58" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="E58" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>262</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>517</v>
       </c>
       <c r="D59" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>517</v>
       </c>
       <c r="D60" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
       <c r="E60" t="s">
-        <v>268</v>
+        <v>210</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="H60" t="s">
-        <v>271</v>
-      </c>
-      <c r="I60" t="s">
-        <v>270</v>
+        <v>263</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="I60" s="14" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C61" t="s">
-        <v>85</v>
-      </c>
       <c r="D61" t="s">
-        <v>80</v>
+        <v>269</v>
       </c>
       <c r="E61" t="s">
-        <v>79</v>
+        <v>268</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>654</v>
+        <v>357</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>84</v>
+        <v>518</v>
       </c>
       <c r="H61" t="s">
-        <v>83</v>
+        <v>271</v>
       </c>
       <c r="I61" t="s">
-        <v>82</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D62" t="s">
+        <v>80</v>
+      </c>
       <c r="E62" t="s">
+        <v>79</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>52</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E63" t="s">
         <v>340</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F63" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="G62" s="10"/>
-    </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="I65" t="s">
-        <v>493</v>
-      </c>
+      <c r="G63" s="10"/>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I66" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I67" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
         <v>495</v>
-      </c>
-    </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
-        <v>116</v>
-      </c>
-      <c r="I68" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
+        <v>116</v>
+      </c>
+      <c r="I69" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
         <v>64</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I70" t="s">
         <v>497</v>
-      </c>
-    </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D70" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="I70" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D71" s="11" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="I71" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D72" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
+      </c>
+      <c r="I72" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D73" s="11" t="s">
-        <v>346</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D74" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D75" s="11" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>247</v>
-      </c>
-      <c r="F76" t="s">
-        <v>345</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
+        <v>247</v>
+      </c>
+      <c r="F77" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
+    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
+    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
         <v>301</v>
       </c>
     </row>
@@ -6688,7 +6728,7 @@
     <sortCondition descending="1" ref="O5"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B62">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B63">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -6704,7 +6744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -7461,7 +7501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -8150,7 +8190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8316,7 +8356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Doing Green lake and some balance ITems/people with Erik
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="685">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2554,6 +2554,12 @@
     <t>Polish 1</t>
   </si>
   <si>
+    <t>EPTA is at 4600 Lines of code!</t>
+  </si>
+  <si>
+    <t>2 - 2 hr Adding more juicy responses, debugging parser more, and documentating parser</t>
+  </si>
+  <si>
     <t>* Add accepting for each senario
 go _
  &lt;objects&gt;, /interacts/, and [people]
@@ -2574,13 +2580,27 @@
 attack _
  &lt;objects&gt;, /interacts/, and [people]
 * Implement feedback
-*Playtests?</t>
-  </si>
-  <si>
-    <t>EPTA is at 4600 Lines of code!</t>
-  </si>
-  <si>
-    <t>2 - 2 hr Adding more juicy responses, debugging parser more, and documentating parser</t>
+*Playtests?
+* get rid of full kit at the start
+ helm of orin bearclaw
+get rid of mdcl
+ wall there
+this looks sharper than this
+ health status
+shutdown your computer from the game
+Reward for 100%
+ Score
+*If put name as big hitz twofer you're invincable 
+*all interactables should do SOMETHING to not lead on
+ at least give you something
+ lamp
+ red book
+ blue book
+*Bug where if you look at lake painting doesn't do thing
+Can't talk to Fred or do anything at green lake properly?</t>
+  </si>
+  <si>
+    <t>4 - 3hr putting Fred and green lake in the game, doing some item and boss balancing</t>
   </si>
 </sst>
 </file>
@@ -3309,7 +3329,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3612,18 +3632,18 @@
         <v>678</v>
       </c>
       <c r="F17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G17" t="s">
         <v>634</v>
       </c>
       <c r="I17" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>635</v>
+        <v>684</v>
       </c>
       <c r="B18" t="s">
         <v>636</v>
@@ -4886,8 +4906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5380,7 +5400,7 @@
         <v>680</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>500</v>

</xml_diff>

<commit_message>
helping Tyler Develop haunted woods, writing code, developing interactables to be able to place anything (equip, person, interact), bits of polishing
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="686">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2560,6 +2560,12 @@
     <t>2 - 2 hr Adding more juicy responses, debugging parser more, and documentating parser</t>
   </si>
   <si>
+    <t>4 - 3hr putting Fred and green lake in the game, doing some item and boss balancing</t>
+  </si>
+  <si>
+    <t>5 - 5.0 hr helping Tyler Develop haunted woods, writing code, developing interactables to be able to place anything (equip, person, interact), bits of polishing</t>
+  </si>
+  <si>
     <t>* Add accepting for each senario
 go _
  &lt;objects&gt;, /interacts/, and [people]
@@ -2597,10 +2603,20 @@
  red book
  blue book
 *Bug where if you look at lake painting doesn't do thing
-Can't talk to Fred or do anything at green lake properly?</t>
-  </si>
-  <si>
-    <t>4 - 3hr putting Fred and green lake in the game, doing some item and boss balancing</t>
+Can't talk to Fred or do anything at green lake properly?
+have a score with a percentage completed!
+test multiple accepts on Fred (they give different things depending on order)
+ability for interacts to place interacts
+place down an interactable and be transformable
+Stage 1
+() is a tuple that can update any item in the game dictionary
+[] is a multiple input ordered list of input and output
+Attribute so that it resets itself
+can set some of it's own attri
+each dimension size is defined in a dictionary of dimensions as the range values
+ get rid of size aspect? Yeah I guess so 
+have a catigory filter in the CSV creator so it's a collumn in the csv, then puts in good order, maybe multiple
+Also would be sick to have a map creator based on tab or maybe just dimension delimiter</t>
   </si>
 </sst>
 </file>
@@ -3328,8 +3344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,10 +3659,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>683</v>
+      </c>
+      <c r="B18" t="s">
         <v>684</v>
-      </c>
-      <c r="B18" t="s">
-        <v>636</v>
       </c>
       <c r="C18" t="s">
         <v>637</v>
@@ -4906,7 +4922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -5400,7 +5416,7 @@
         <v>680</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>500</v>

</xml_diff>

<commit_message>
Made changes to HF
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -2781,36 +2781,37 @@
 </t>
   </si>
   <si>
-    <t>11 - 3.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending,</t>
+    <t>11 - 4.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest,</t>
   </si>
   <si>
     <t>*1. BugFix
 *1.5 Spelling
 Check spelling of the game
-*2. Playtest/balance
-- [ ] still a problem with layers, saving and loading, hope it works for 0.27 release
-- [ ] Can't play as tyler Kashak after you stop
-- [ ] Check to make sure nest game, correct times, and everything add up
-Need some sort of text descriptions, even if it's just to say one thing looks better.
-Need to play through and see if we can beat without secrets - Erik
-Play the hek out of forest, green lake, all quests, etc
-If needed for balancing write the fight simulator script
-Make the PAP unlock, scoring, and the 100% meter
-*3. GUI
+*1.7 Quick Playthrough
+0.5 See if playing through gameworks
+*2. GUI
 Make read speed changable or maybe even skipable within printT keyboard interrupt
 Make the descriptions line up
 Make ingame settings with changeable: read speed, colour
 Scaleable Ascii Art
 PrintT (if no items there's large spacing, search if no items gives weird cutoff? (but it's not the same as moving into the spot, need to standardize this))
     Make the search standard part of the function and use the general move one as it seems to be correct.
+Make the MAP.SEARCH function encapsulating and control everything like if you wake up there or not, etc
 Colours are still sometimes glitchy
+*3. Features
+Need some sort of text descriptions, even if it's just to say one thing looks better.
+Need to play through and see if we can beat without secrets - Erik
+If needed for balancing write the fight simulator script
+Make the PAP unlock, scoring, and the 100% meter
 *4. Lore
 Add Lore so that everything flows nicer and is more readable
 *5. Content Add
 *Make the Haunted expansion Playable
-The way in cootes says "you knew more about survival so you could go through"
-The RED book is a survival guide to cootes and opens it up
-Blue book is one that is just garabage that says "stay hydrated!"
+Play the hek out of forest, green lake, all quests, etc
+* EPTA All the way down Fixes (doing these last because kin
+- [ ] still a problem with layers, saving and loading, hope it works for 0.27 release
+- [ ] Can't play as tyler Kashak after you stop
+- [ ] Check to make sure nest game, correct times, and everything add up
 *Add feedback Content</t>
   </si>
 </sst>
@@ -3553,7 +3554,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed some parser things
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -2781,9 +2781,6 @@
 </t>
   </si>
   <si>
-    <t>11 - 4.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest,</t>
-  </si>
-  <si>
     <t>*1. BugFix
 *1.5 Spelling
 Check spelling of the game
@@ -2798,6 +2795,7 @@
     Make the search standard part of the function and use the general move one as it seems to be correct.
 Make the MAP.SEARCH function encapsulating and control everything like if you wake up there or not, etc
 Colours are still sometimes glitchy
+Make the places the intuitive names "INFRONT OF" usually means with reference to front of building
 *3. Features
 Need some sort of text descriptions, even if it's just to say one thing looks better.
 Need to play through and see if we can beat without secrets - Erik
@@ -2813,6 +2811,9 @@
 - [ ] Can't play as tyler Kashak after you stop
 - [ ] Check to make sure nest game, correct times, and everything add up
 *Add feedback Content</t>
+  </si>
+  <si>
+    <t>11 - 5.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest, playtesting balance changes,</t>
   </si>
 </sst>
 </file>
@@ -3553,7 +3554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3891,7 +3892,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B19" t="s">
         <v>544</v>
@@ -5131,7 +5132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -5669,7 +5670,7 @@
         <v>693</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="26"/>

</xml_diff>

<commit_message>
Some bugfixes and changes
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -2813,7 +2813,7 @@
 *Add feedback Content</t>
   </si>
   <si>
-    <t>11 - 5.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest, playtesting balance changes,</t>
+    <t xml:space="preserve">11 - 6.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest, playtesting balance changes, </t>
   </si>
 </sst>
 </file>
@@ -3555,7 +3555,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Did lots of tweaks
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="700">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2589,14 +2589,55 @@
     <t>Finish List</t>
   </si>
   <si>
+    <t>10 - 2 hr making final list, fixing some minor bugs and devmode,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
+* PP8 style using PyCharm
+* Get rid of global variables and restructure code
+* Maybe make each class and big function its own module file
+* Using and understanding effecient python code chunks (See Liam F. and his book)
+* Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
+* Map
+So we are making a MUD and I didn't know it LOL
+Better than trying to retrofit everything and then you have unique addressing
+Have a linked exit on the spots beside, no need to go inside or anything, just update position and move around
+Map will just constrain itself by where edges are and where you can move
+* Nevada Game engine
+Graph with adjacency list (stored effeciently) that gives the possible options. 
+Using paths with path constructor to translate between points (instead of on-command search). Then maps just become entities addresses by the name.
+For destruction just do pointer to point all old places to the new place (but does damage/kill people when you do destroy a spot)
+* Entity
+     Person(each has same attributes and stuff, even schedule would be the same)
+          Boss?
+     Place
+          Interroor
+     Item
+          Interactable
+          Interactable can go, just add a moveable flag to items with new entity structute that allows give/take
+* Have a generalized interface class/objects so you don't have to make new ones every time
+* Calling it Mac Quest? McMaster MUD? MMUD
+* See TODO list for rest of rebuild notes
+* Follow a structure like in pygame where exiting game loop sets you back to game menu, etc
+* Upgrade python to python3 using py2to3
+*Overhaul interacables, items, and enemies so they more versatilie (can drop anything, update the dictionaries, etc)
+**GET RID OF location checking in functions AND location attribute entirely and just use storage lists in each map location (should get rid of duplicate problems AND will go better with adjacency lists probably)
+Player list
+Item list
+Interactables list
+Enemies list (rename enemies to NPCs)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 - 6.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest, playtesting balance changes, </t>
+  </si>
+  <si>
     <t>*Do all polishing in non-dev mode
 *Hollywood Playthrough Feedback
-Scholar's road
 Just use colours for differentiation 
 But can set forground and background if you want
 Option to skip text would be cool, but better to be faster to read and can set read speed. Don't want to be annoyed
 If tavelled there before read should be instant
-Bugs of name of person
 No clear screen of things, easier to scroll up
 Typo on help intro. Grammarly
 Add quest or used flag for items if inspected
@@ -2605,10 +2646,9 @@
 *Playtests?
 this looks sharper than this
  health status
-shutdown your computer from the game
 Reward for 100%
  Score
-*all interactables should do SOMETHING to not lead on
+*all interactables should do SOMETHING to not lead on (at least say you can't do anything with this)
  at least give you something
  lamp
  red book
@@ -2626,7 +2666,6 @@
  get rid of size aspect? Yeah I guess so 
 have a catigory filter in the CSV creator so it's a collumn in the csv, then puts in good order, maybe multiple
 Also would be sick to have a map creator based on tab or maybe just dimension delimiter
-*Dev mode hiding can be as simple as disabling Dev mode before releasing but still have way to get into it through game (e.g. typing in 420e69 or maybe something more complicated and fast to type in)
 ** Game should be immersive through people and things based on what you've done. People talk more about the story of what happened, items reflect what had been done or what for (ex blood on them if you kill someone), and the storyline and progression is talked about (talking more about Kipling and the Phoniex and Quantum order)
 *PrintT might need some more customization for spacing and reading timing
 *Make sure Dev mode is deleted from settings file once saved 
@@ -2646,10 +2685,6 @@
 Enemy infi
 Enemy special info
 *Bugs from playthrough with Erik
--Admin privileges
-Right click run as admin
-Not sure what the colours mean
--Take out Dev mode from settings file
 -In instructions say that the talk and use
 -highlightinf messes up sometimes
 -Ingame settings to change settings
@@ -2741,51 +2776,12 @@
 CHANGED Colours now much better and keep when there's an empty room</t>
   </si>
   <si>
-    <t>10 - 2 hr making final list, fixing some minor bugs and devmode,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
-* PP8 style using PyCharm
-* Get rid of global variables and restructure code
-* Maybe make each class and big function its own module file
-* Using and understanding effecient python code chunks (See Liam F. and his book)
-* Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
-* Map
-So we are making a MUD and I didn't know it LOL
-Better than trying to retrofit everything and then you have unique addressing
-Have a linked exit on the spots beside, no need to go inside or anything, just update position and move around
-Map will just constrain itself by where edges are and where you can move
-* Nevada Game engine
-Graph with adjacency list (stored effeciently) that gives the possible options. 
-Using paths with path constructor to translate between points (instead of on-command search). Then maps just become entities addresses by the name.
-For destruction just do pointer to point all old places to the new place (but does damage/kill people when you do destroy a spot)
-* Entity
-     Person(each has same attributes and stuff, even schedule would be the same)
-          Boss?
-     Place
-          Interroor
-     Item
-          Interactable
-          Interactable can go, just add a moveable flag to items with new entity structute that allows give/take
-* Have a generalized interface class/objects so you don't have to make new ones every time
-* Calling it Mac Quest? McMaster MUD? MMUD
-* See TODO list for rest of rebuild notes
-* Follow a structure like in pygame where exiting game loop sets you back to game menu, etc
-* Upgrade python to python3 using py2to3
-*Overhaul interacables, items, and enemies so they more versatilie (can drop anything, update the dictionaries, etc)
-**GET RID OF location checking in functions AND location attribute entirely and just use storage lists in each map location (should get rid of duplicate problems AND will go better with adjacency lists probably)
-Player list
-Item list
-Interactables list
-Enemies list (rename enemies to NPCs)
-</t>
+    <t>12 - 4 hr played through and made quest/acheivment list, fixing save file, fixing colours, dealing with garbage expansion</t>
   </si>
   <si>
     <t>*1. BugFix
 *1.5 Spelling
 Check spelling of the game
-*1.7 Quick Playthrough
-0.5 See if playing through gameworks
 *2. GUI
 Make read speed changable or maybe even skipable within printT keyboard interrupt
 Make the descriptions line up
@@ -2796,24 +2792,38 @@
 Make the MAP.SEARCH function encapsulating and control everything like if you wake up there or not, etc
 Colours are still sometimes glitchy
 Make the places the intuitive names "INFRONT OF" usually means with reference to front of building
+HIGHLIGHT words in the description as well (even if not changeable)
+Maybe use highlighting to show if things are better
+Dropped things from interacables or enemies have no colour
 *3. Features
 Need some sort of text descriptions, even if it's just to say one thing looks better.
-Need to play through and see if we can beat without secrets - Erik
-If needed for balancing write the fight simulator script
-Make the PAP unlock, scoring, and the 100% meter
+Make the PAP unlock, scoring, and the 100% meter, acheivements
 *4. Lore
 Add Lore so that everything flows nicer and is more readable
 *5. Content Add
 *Make the Haunted expansion Playable
 Play the hek out of forest, green lake, all quests, etc
+'DrOWN I Need EveryThing graBs' 
+ -doesn't apply anymore, basement of ETB doesn't have anything useful
+When you enter a load game, a "search" command should autorun in order to reintroduce you to your surroundings
+Old car keys don't open old car... :(
+One of the walls in the maze is still a "one-way only"
+ -two squares to the left of the wolf
+ -should be a dead end, only path to the left
+typo:
+"your leg...\You must be seeing things..."
+"start to
+at the ba"
+Bad discription:
+"HEAVY ROCK
+It is a stick found in the forest."
+Bad naming:
+log + kindling = "Lit Firepit" ???
 * EPTA All the way down Fixes (doing these last because kin
 - [ ] still a problem with layers, saving and loading, hope it works for 0.27 release
 - [ ] Can't play as tyler Kashak after you stop
 - [ ] Check to make sure nest game, correct times, and everything add up
 *Add feedback Content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 - 6.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest, playtesting balance changes, </t>
   </si>
 </sst>
 </file>
@@ -3554,8 +3564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3887,15 +3897,15 @@
         <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
+        <v>696</v>
+      </c>
+      <c r="B19" t="s">
         <v>698</v>
-      </c>
-      <c r="B19" t="s">
-        <v>544</v>
       </c>
       <c r="C19" t="s">
         <v>545</v>
@@ -5132,8 +5142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5626,7 +5636,7 @@
         <v>676</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>498</v>
@@ -5670,7 +5680,7 @@
         <v>693</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="26"/>
@@ -6919,7 +6929,7 @@
         <v>79</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Haunted Forest Should be Done
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -2776,29 +2776,23 @@
 CHANGED Colours now much better and keep when there's an empty room</t>
   </si>
   <si>
-    <t>12 - 4 hr played through and made quest/acheivment list, fixing save file, fixing colours, dealing with garbage expansion</t>
-  </si>
-  <si>
     <t>*1. BugFix
 *1.5 Spelling
 Check spelling of the game
 *2. GUI
-Make read speed changable or maybe even skipable within printT keyboard interrupt
+Make the places the intuitive names "INFRONT OF" usually means with reference to front of building
 Make the descriptions line up
-Make ingame settings with changeable: read speed, colour
+Make the MAP.SEARCH function encapsulating and control everything like if you wake up there or not, etc
+Dropped things from interacables or enemies have no colour
+Make ingame settings with changeable: read speed, background, text colour, or maybe even skipable within printT keyboard interrupt
 Scaleable Ascii Art
 PrintT (if no items there's large spacing, search if no items gives weird cutoff? (but it's not the same as moving into the spot, need to standardize this))
     Make the search standard part of the function and use the general move one as it seems to be correct.
-Make the MAP.SEARCH function encapsulating and control everything like if you wake up there or not, etc
 Colours are still sometimes glitchy
-Make the places the intuitive names "INFRONT OF" usually means with reference to front of building
-HIGHLIGHT words in the description as well (even if not changeable)
-Maybe use highlighting to show if things are better
-Dropped things from interacables or enemies have no colour
 *3. Features
-Need some sort of text descriptions, even if it's just to say one thing looks better.
 Make the PAP unlock, scoring, and the 100% meter, acheivements
 *4. Lore
+HIGHLIGHT words in the description as well (even if not changeable)
 Add Lore so that everything flows nicer and is more readable
 *5. Content Add
 *Make the Haunted expansion Playable
@@ -2824,6 +2818,9 @@
 - [ ] Can't play as tyler Kashak after you stop
 - [ ] Check to make sure nest game, correct times, and everything add up
 *Add feedback Content</t>
+  </si>
+  <si>
+    <t>12 - 6 hr played through and made quest/acheivment list, fixing save file, fixing colours, dealing with garbage expansion, adding text descriptions of health, adding text descriptions of items, putting in HF rewards</t>
   </si>
 </sst>
 </file>
@@ -3564,8 +3561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3905,7 +3902,7 @@
         <v>696</v>
       </c>
       <c r="B19" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C19" t="s">
         <v>545</v>
@@ -4112,7 +4109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="F44" workbookViewId="0">
+    <sheetView topLeftCell="F20" workbookViewId="0">
       <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
@@ -5142,8 +5139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5680,7 +5677,7 @@
         <v>693</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="26"/>

</xml_diff>

<commit_message>
HOW IS GAME BROKEN
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -30,18 +30,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="703">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2545,29 +2539,6 @@
     <t>More expansion but hard to find</t>
   </si>
   <si>
-    <t>Need to implement entrance to the area
-Need to implement entrance to the cabin, also the link
-Need auto descriptions to work with interriors
-Make sure stick duplicates doesn't cause any problems, OH IT totally will because dictionary has unique keys
-       Make some way that sticks display similarly or that the interact accepts any of the sticks
-Mit says "It looks to be child sized."
-Having farming guy roam through the forest once he's mad
-The Greif attribute with the little girl
-Check to see if needed on enemy that it doesn't give you anything until you kill them
-Done:
-*ADDED WHOLE NEW 10X10 AREA WITH NEW QUESTS, ITEMS, CHARACTERS, ETC to startup
-*CHANNGED Interactables can now drop Items, Interacts, or People!
-*ADDED Secret/Dev Area of Green lake that you need keys to get into
-*ADDED Rules for writing objects in startup:
-0. ALWAYS check the paramaters of the object. If unsure check GameClasses.py for the constructor
-1. Use " (\S)" instead of "\n" for newline characters
-2. If using ANY quotes (" or ') ONLY use ' inside strings.
-The " quote is used to define the string boundry and any in the sentence will break the string.
-ex) "You think to yourself 'Gee, do I like quotes'! 'Lets go somewhere!' "
-not) "You think to yourself "Gee, do I like quotes"! "Lets go somewhere"! "
-3. When an attribute is none it needs to be capitalized as such: None</t>
-  </si>
-  <si>
     <t>* 3BB PID with MSP430
 MSP430 into piezoelectric cooler, now need PID system
 * Giving context about 3W text and also have more things tell you about phoneix and also items (More use of storyline, music, definition to people to give realism to the world)
@@ -2632,45 +2603,56 @@
     <t xml:space="preserve">11 - 6.5 hr Putting data and savepath in %Appdata%/Roaming, fixed the empty file showing, fixed the name change character bugs, added game info display, scripts can now be run again!, fixing quest bugs and creating neutral ending, imp. Haunted forest, playtesting balance changes, </t>
   </si>
   <si>
+    <t>12 - 10 hr played through and made quest/acheivment list, fixing save file, fixing colours, dealing with garbage expansion, adding text descriptions of health, adding text descriptions of items, putting in HF rewards, idk what I'm doing now, fixing description spacing, fixing colouring, making search better, fixing direction alignment cause insane, fixing bugs</t>
+  </si>
+  <si>
+    <t>Having farming guy roam through the forest once he's mad
+The Greif attribute with the little girl
+Check to see if needed on enemy that it doesn't give you anything until you kill them
+Done:
+*ADDED WHOLE NEW 10X10 AREA WITH NEW QUESTS, ITEMS, CHARACTERS, ETC to startup
+*CHANNGED Interactables can now drop Items, Interacts, or People!
+*ADDED Secret/Dev Area of Green lake that you need keys to get into
+*ADDED Rules for writing objects in startup:
+0. ALWAYS check the paramaters of the object. If unsure check GameClasses.py for the constructor
+1. Use " (\S)" instead of "\n" for newline characters
+2. If using ANY quotes (" or ') ONLY use ' inside strings.
+The " quote is used to define the string boundry and any in the sentence will break the string.
+ex) "You think to yourself 'Gee, do I like quotes'! 'Lets go somewhere!' "
+not) "You think to yourself "Gee, do I like quotes"! "Lets go somewhere"! "
+3. When an attribute is none it needs to be capitalized as such: None</t>
+  </si>
+  <si>
+    <t>*1. BugFix
+*1.5 Spelling
+Check spelling of the game
+*2. GUI
+Make ingame settings with changeable: read speed, background, text colour, or maybe even skipable within printT keyboard interrupt
+Scaleable Ascii Art
+PrintT is still weird
+*3. Features
+Make the PAP unlock, scoring, and the 100% meter, acheivements file with highest percentage
+*4. Lore
+HIGHLIGHT words in the description as well (even if not changeable)
+Add Lore so that everything flows nicer and is more readable
+* For game lore give hints to where profs would be before they actually spawn
+*5. Content Add
+*Make the Haunted expansion Playable
+Play the hek out of forest, green lake, all quests, etc
+* EPTA All the way down Fixes (doing these last because kin
+- [ ] still a problem with layers, saving and loading, hope it works for 0.27 release
+- [ ] Can't play as tyler Kashak after you stop
+- [ ] Check to make sure nest game, correct times, and everything add up
+*Add feedback Content</t>
+  </si>
+  <si>
     <t>*Do all polishing in non-dev mode
 *Hollywood Playthrough Feedback
-Just use colours for differentiation 
-But can set forground and background if you want
 Option to skip text would be cool, but better to be faster to read and can set read speed. Don't want to be annoyed
-If tavelled there before read should be instant
-No clear screen of things, easier to scroll up
 Typo on help intro. Grammarly
 Add quest or used flag for items if inspected
-Make events so they're reoccurring
-Don't need interrupts but need dimensions for spooky  shortcut
-*Playtests?
-this looks sharper than this
- health status
-Reward for 100%
- Score
-*all interactables should do SOMETHING to not lead on (at least say you can't do anything with this)
- at least give you something
- lamp
- red book
- blue book
-have a score with a percentage completed!
-test multiple accepts on Fred (they give different things depending on order)
-ability for interacts to place interacts
-place down an interactable and be transformable
-Stage 2 Interacts
-() is a tuple that can update any item in the game dictionary
-[] is a multiple input ordered list of input and output
-Attribute so that it resets itself
-can set some of it's own attri
-each dimension size is defined in a dictionary of dimensions as the range values
- get rid of size aspect? Yeah I guess so 
-have a catigory filter in the CSV creator so it's a collumn in the csv, then puts in good order, maybe multiple
-Also would be sick to have a map creator based on tab or maybe just dimension delimiter
 ** Game should be immersive through people and things based on what you've done. People talk more about the story of what happened, items reflect what had been done or what for (ex blood on them if you kill someone), and the storyline and progression is talked about (talking more about Kipling and the Phoniex and Quantum order)
 *PrintT might need some more customization for spacing and reading timing
-*Make sure Dev mode is deleted from settings file once saved 
-Also setting file should not be able to be opened while played, maybe just hidden in cache
-*BUG If you exit game it crashes causing the flag!
 *A spell check thing that printTs out everything for spell checking
 All things from the start/loading/response
 All quest stuff
@@ -2685,65 +2667,15 @@
 Enemy infi
 Enemy special info
 *Bugs from playthrough with Erik
--In instructions say that the talk and use
--highlightinf messes up sometimes
--Ingame settings to change settings
--reading Is too slow?
--dont have the opening clear screen so it says what do you want to do incase you don't finish reading?
-- infront of BSB and behind BSB is confusing 
-Could do in relation to where the front of the building is or could do "BESIDE"
-Should be infront of JHE from the perspective of the building
-- if you try give something to someone 
--it should be more apparent when stuff is strong
-Maybe colours, maybe text descriptions, easy thing would be to say that it's very strong. Another thing is to say that the more you help people the stronger rewards you will get
-- search speed is good for revisit, maybe if you do run it is instant (ru) 
-- Wool sweater should be marina wool
-- dialogue that says taking 3 mayo jars
-Next more 
--  get rid of windshield people dialogue
-- be able to eat a pizza box
 - don't do blue highlighting for quests
-- the flavour descriptions with key words should b pickable so that you point them towards the area/thing you want them to look at
 - hint system with consumeable to point out a hint to  the person
 - if you wait in the room long enough it will give you a hint, get a reminder on your phone
 Having something in game to get stuck in an area
-- What is an old lamp?
-- the colour of the item when something is dropped on yhe ground 
-- writing is awesome!
 - GitHub in work environment push small and frequently
-- Have Rod want to get his climbing shoes not the bowling ball
-- add a score to have things and show in stats
 - idea: definistate threw window
-- Conor doesn't give any rewards
-- doesn't say completionist and unlocks stuff
-- talk shovel
-- is indepence storyline finished?
 - have sub basement  in ETB so Tarzan goes down
-- have someone need the potato
-- secret room isn't visible until you 
-- magnesium spelled wrong, get rid of red-blue-green and label 1,2,3
-- highlighting sometimes messes up
-*Add 2-3 extra parameters in objects that are empty
-*Make score, secrets used, and speedrun be recorded in game
 *Erik Feedback:
-Bleach squirt bottle colour (colour of items when they're dropped and all interactions
-declaration of independence colour
-Vomit colour
-Femtosecond Laser colour
-why does rr and dd send you up? (maybe have no spell checking on two letter words either)
-"The first game to indroduce" "A fine game but defiently"
-"Mangnesium"  (Spelling mistakes)
 looking into blue pool in the basement of the reactor?? When your in the basement you can't see any pool, it's from the main floor you see the glow. (Okay we can change this)
-giving connor the cricket has no reward :( (okay I think he does now)
-"use femtosecond laser" doesnt work, have to pick it up first (same with relativistic key)  (picking up from floor a thing)
-* Empty Game Still Loads
-* For game lore give hints to where profs would be before they actually spawn
-* Have the colour in the lore to highlight certain words
-* Polish the auto directions in all cases
-tab to line up
-[F] Forest      [L] Forest      [R] Forest on same line
-[U] 2nd Floor W Wing    [F] T-13        [B] Hospital East Wing
-* Wacky items are good
 Nice to have:
 *Remove Archway and put university hall, 
 then implementing using dimension dictionary and add if you try to move out of bounds of dimension it says 'you're compelled to stay within'
@@ -2776,48 +2708,13 @@
 CHANGED Colours now much better and keep when there's an empty room</t>
   </si>
   <si>
-    <t>12 - 10 hr played through and made quest/acheivment list, fixing save file, fixing colours, dealing with garbage expansion, adding text descriptions of health, adding text descriptions of items, putting in HF rewards, idk what I'm doing now, fixing description spacing, fixing colouring, making search better, fixing direction alignment cause insane, fixing bugs</t>
-  </si>
-  <si>
-    <t>13 - Add attributes for next game +QA Reading, QA Spelling, QA Release, Release</t>
-  </si>
-  <si>
-    <t>*1. BugFix
-*1.5 Spelling
-Check spelling of the game
-*2. GUI
-Make ingame settings with changeable: read speed, background, text colour, or maybe even skipable within printT keyboard interrupt
-Scaleable Ascii Art
-PrintT is still weird
-*3. Features
-Make the PAP unlock, scoring, and the 100% meter, acheivements file with highest percentage
-*4. Lore
-HIGHLIGHT words in the description as well (even if not changeable)
-Add Lore so that everything flows nicer and is more readable
-*5. Content Add
-*Make the Haunted expansion Playable
-Play the hek out of forest, green lake, all quests, etc
-'DrOWN I Need EveryThing graBs' 
- -doesn't apply anymore, basement of ETB doesn't have anything useful
-When you enter a load game, a "search" command should autorun in order to reintroduce you to your surroundings
-Old car keys don't open old car... :(
-One of the walls in the maze is still a "one-way only"
- -two squares to the left of the wolf
- -should be a dead end, only path to the left
-typo:
-"your leg...\You must be seeing things..."
-"start to
-at the ba"
-Bad discription:
-"HEAVY ROCK
-It is a stick found in the forest."
-Bad naming:
-log + kindling = "Lit Firepit" ???
-* EPTA All the way down Fixes (doing these last because kin
-- [ ] still a problem with layers, saving and loading, hope it works for 0.27 release
-- [ ] Can't play as tyler Kashak after you stop
-- [ ] Check to make sure nest game, correct times, and everything add up
-*Add feedback Content</t>
+    <t xml:space="preserve">13 - 1hr </t>
+  </si>
+  <si>
+    <t>QA Reading, :QA Reading, QA Spelling, QA Release, Release</t>
+  </si>
+  <si>
+    <t>14 - 5 hr added aesthetic classes, did some documention, did some colouring, trying to aesthetics, HUGE bugfix on printT counting ansii escape characters fixed, QA spelling+grammar+immersiveness</t>
   </si>
 </sst>
 </file>
@@ -3558,8 +3455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,7 +3779,7 @@
         <v>635</v>
       </c>
       <c r="D18" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E18" t="s">
         <v>541</v>
@@ -3891,21 +3788,21 @@
         <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
+        <v>695</v>
+      </c>
+      <c r="B19" t="s">
         <v>696</v>
       </c>
-      <c r="B19" t="s">
-        <v>698</v>
-      </c>
       <c r="C19" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D19" t="s">
-        <v>613</v>
+        <v>702</v>
       </c>
       <c r="E19" t="s">
         <v>614</v>
@@ -3915,6 +3812,11 @@
       </c>
       <c r="G19" t="s">
         <v>616</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -5136,8 +5038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5505,7 +5407,7 @@
         <v>408</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G12" t="s">
         <v>498</v>
@@ -5630,7 +5532,7 @@
         <v>676</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>498</v>
@@ -5649,7 +5551,7 @@
         <v>688</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>690</v>
+        <v>697</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>498</v>
@@ -5671,10 +5573,10 @@
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="26"/>
@@ -6923,7 +6825,7 @@
         <v>79</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
I did everything I could. Still couldn't get saves to work so just implemented the scripter for the loadgame :)
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="711">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -2711,10 +2711,34 @@
     <t xml:space="preserve">13 - 1hr </t>
   </si>
   <si>
-    <t>QA Reading, :QA Reading, QA Spelling, QA Release, Release</t>
-  </si>
-  <si>
-    <t>14 - 5 hr added aesthetic classes, did some documention, did some colouring, trying to aesthetics, HUGE bugfix on printT counting ansii escape characters fixed, QA spelling+grammar+immersiveness</t>
+    <t>for each file that prints something:</t>
+  </si>
+  <si>
+    <t>check spelling + grammar</t>
+  </si>
+  <si>
+    <t>colouring of outputs</t>
+  </si>
+  <si>
+    <t>check immersiveness</t>
+  </si>
+  <si>
+    <t>make it use printT instead of print</t>
+  </si>
+  <si>
+    <t>CHANGE .name to colouredname</t>
+  </si>
+  <si>
+    <t>Check the start.py last after doing FULL playthrough and adding immersive aesthetic objects</t>
+  </si>
+  <si>
+    <t>6f8202378e2b91fdd632c4adbef05ec1894edfe9</t>
+  </si>
+  <si>
+    <t>14 - 8 hr added aesthetic classes, did some documention, did some colouring, trying to aesthetics, HUGE bugfix on printT counting ansii escape characters fixed, debugging, playing, god it's 12:40.</t>
+  </si>
+  <si>
+    <t>Plaything through EVERYTHING till finish and debug anything you find</t>
   </si>
 </sst>
 </file>
@@ -3453,7 +3477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -3742,7 +3766,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>670</v>
       </c>
@@ -3768,7 +3792,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>679</v>
       </c>
@@ -3790,8 +3814,11 @@
       <c r="G18" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>695</v>
       </c>
@@ -3802,7 +3829,7 @@
         <v>700</v>
       </c>
       <c r="D19" t="s">
-        <v>702</v>
+        <v>709</v>
       </c>
       <c r="E19" t="s">
         <v>614</v>
@@ -3814,17 +3841,48 @@
         <v>616</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>710</v>
+      </c>
+      <c r="N20" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>637</v>
       </c>
@@ -3853,7 +3911,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>613</v>
       </c>
@@ -3882,7 +3940,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>621</v>
       </c>
@@ -3911,7 +3969,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>639</v>
       </c>
@@ -4001,6 +4059,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed some highlighting and fixed keyerror
</commit_message>
<xml_diff>
--- a/Dev/EPTA Developent Roadmap.xlsx
+++ b/Dev/EPTA Developent Roadmap.xlsx
@@ -2753,7 +2753,7 @@
     <t>19 - 1 hr pygaming reading</t>
   </si>
   <si>
-    <t>19 - 2 hr QA and highlighting</t>
+    <t>19 - 3.5 hr QA and highlighting, social media</t>
   </si>
 </sst>
 </file>
@@ -3495,7 +3495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>